<commit_message>
chore: update 128 sem1 tt
</commit_message>
<xml_diff>
--- a/raw/time_tables/B.Tech 128 (btech-128)/1/1.xlsx
+++ b/raw/time_tables/B.Tech 128 (btech-128)/1/1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="595">
   <si>
     <t>B.TECH. I Yr(I SEMESTER) TIMETABLE ODD SEMESTER 2025, JIIT-128</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>TE4(15B11CI1111) -116/TWT</t>
-  </si>
-  <si>
-    <t>TF9(24B11EC111)-116/KUM</t>
   </si>
   <si>
     <t>TH2(15B11MA111)-116
@@ -74,19 +71,19 @@
     <t>TH1(24B11EC111)-121/BAB</t>
   </si>
   <si>
-    <t>TF17(24B11EC111)-116//RAV</t>
+    <t>TF17(24B11EC111)-116//RPV</t>
   </si>
   <si>
     <t>PF7F8F9(24B15CS111) - /CL1/AKB/SHG/NIB</t>
   </si>
   <si>
-    <t>PF16(15B1HS112) -/240/DV</t>
+    <t>PF18(15B1HS112) -/240/DEV</t>
   </si>
   <si>
     <t>PF1(24B15EC111)-/BE LAB-I/BHC</t>
   </si>
   <si>
-    <t>PF21(15B1HS112)-240/MEENAKSHI</t>
+    <t>PF21(15B1HS112)-240/MEENAKSHI/AARUSHI</t>
   </si>
   <si>
     <t>PF3(15B17PH171) - /41/ADV/ANK</t>
@@ -107,23 +104,23 @@
     <t>LH1H2(15B11PH111) -SR05/SKA</t>
   </si>
   <si>
-    <t>LE3E4(24B11EC111)) -123/MAG</t>
-  </si>
-  <si>
-    <t>PE3(24B15EC111)/DE LAB/JMN</t>
+    <t>LE3E4(24B11EC111)) -123/MEA</t>
+  </si>
+  <si>
+    <t>PE3(24B15EC111)/DE LAB/AJK</t>
   </si>
   <si>
     <t>LF13F14(15B11PH111) -118/NAK</t>
   </si>
   <si>
-    <t>LF16F17(15B11MA111)-117
-/NFMATH4</t>
-  </si>
-  <si>
-    <t>LF16F17(15B11PH111) -117/BHT</t>
-  </si>
-  <si>
-    <t>TF25(24B11EC111) -126/NFEC1</t>
+    <t>LF18F17(15B11MA111)-117
+/ASP</t>
+  </si>
+  <si>
+    <t>LF18F17(15B11PH111) -117/BHT</t>
+  </si>
+  <si>
+    <t>TF25(24B11EC111) -126/RAS</t>
   </si>
   <si>
     <t>PF1F2F21(18B15GE111)/EDD/CADD03/PRJ/HAB/NIK</t>
@@ -134,13 +131,13 @@
   </si>
   <si>
     <t>LE1E2(15B11MA111)-SR05
-/NFMATHS4</t>
+/SHP</t>
   </si>
   <si>
     <t>PF3F4F22(18B15GE111)/EDD/CADD03/SUM/PSH/RAK/JUGENDRA SINGH</t>
   </si>
   <si>
-    <t>PF5(15B1HS112)-/240/ANB</t>
+    <t>PF5(15B1HS112)-/240/EKS</t>
   </si>
   <si>
     <t>PH1(15B1HS112)-/246/HIMANSHI</t>
@@ -152,9 +149,6 @@
     <t>PE3(15B17PH171)-41/ADV/NFPHY3</t>
   </si>
   <si>
-    <t>TF6(15B11PH111)-121/URS</t>
-  </si>
-  <si>
     <t>PF4(15B17PH171)-/027/VM/NFPHY3</t>
   </si>
   <si>
@@ -170,13 +164,13 @@
     <t>PE1(15B1HS112)-/246/NIC</t>
   </si>
   <si>
-    <t>PH2(24B15EC111)/BE LAB-I/ABK</t>
-  </si>
-  <si>
-    <t>LF7F8(15B11CI1111) -111 /HIA</t>
-  </si>
-  <si>
-    <t>PF6(24B15EC111)/BE LAB-I/SVS</t>
+    <t>PH2(24B15EC111)/BE LAB-II/ABK</t>
+  </si>
+  <si>
+    <t>LF7F8(15B11CI1111) -111 /HIB</t>
+  </si>
+  <si>
+    <t>PF6(24B15EC111)/BE LAB-I/AJK</t>
   </si>
   <si>
     <t>LF9F10(15B11MA111)-118
@@ -195,7 +189,7 @@
     <t>PF10(24B15EC111)/BE LAB-II/NIY</t>
   </si>
   <si>
-    <t>LE1E2(15B11CI1111) -123 /NFCS5</t>
+    <t>LE1E2(15B11CI1111) -123 /RISHAB</t>
   </si>
   <si>
     <t>LF24F25(15B11PH111) -
@@ -213,63 +207,63 @@
   </si>
   <si>
     <t>LF13F14(15B11MA111)-
-111/NFMATH3</t>
+111/SHP</t>
   </si>
   <si>
     <t>LF3F4(15B11MA111)-117
 /MSZ</t>
   </si>
   <si>
-    <t>PF8(15B1HS112) - 240/HIMANSHI</t>
-  </si>
-  <si>
-    <t>LF16F17(24B11EC111) - 118/RPV</t>
-  </si>
-  <si>
-    <t>LF16F17(15B11CI1111) -118 /TKW</t>
+    <t>PF8(15B1HS112) - 240/ANB</t>
+  </si>
+  <si>
+    <t>LF18F17(24B11EC111) - 118/RPV</t>
+  </si>
+  <si>
+    <t>LF18F17(15B11CI1111) -118 /MOHIT</t>
   </si>
   <si>
     <t>LF13F14(24B11EC111) -111 /ATK</t>
   </si>
   <si>
     <t>LE1E2(24B11EC111) -SR05 
-/JMN</t>
-  </si>
-  <si>
-    <t>TF5(15B11PH111)-127/ADV</t>
-  </si>
-  <si>
-    <t>TE2(24B11EC111) -116/JMN</t>
+/PRK</t>
+  </si>
+  <si>
+    <t>LE1E2(15B11HS112) -SR05/NIC</t>
+  </si>
+  <si>
+    <t>TE2(24B11EC111) -116/PRK</t>
   </si>
   <si>
     <t>LH3H4(15B11PH111) -SR05/BHARTI</t>
   </si>
   <si>
-    <t>TF22(24B11EC111)-126/RAV</t>
+    <t>TF22(24B11EC111)-126/RPV</t>
   </si>
   <si>
     <t>TF5(15B11CI1111) -126/SHM</t>
   </si>
   <si>
-    <t>TH4(15B11MA111)-113
+    <t>TH4(15B11MA111)-118
 /PKR</t>
   </si>
   <si>
     <t>TH2(15B11CI1111) -121/GAH</t>
   </si>
   <si>
-    <t>TF5(24B11EC111)-127/SVS</t>
+    <t>TF5(24B11EC111)-127/PRK</t>
   </si>
   <si>
     <t>TH3(15B11MA111)-127
 /PKR</t>
   </si>
   <si>
-    <t>PF24(24B15EC111) -/DE LAB/NFEC1</t>
+    <t>PF24(24B15EC111) -/DE LAB/RAS</t>
   </si>
   <si>
     <t>LF24F25(24B11EC111) -123
-/NFEC1</t>
+/RAS</t>
   </si>
   <si>
     <t>TUESDAY</t>
@@ -306,7 +300,7 @@
     <t>PF9(15B17PH171)-41/URS/NFPHY3</t>
   </si>
   <si>
-    <t>TF24(24B11EC111) -126/NFEC1</t>
+    <t>TF24(24B11EC111) -126/RAS</t>
   </si>
   <si>
     <t>LF1F2(15B11MA111)-148
@@ -321,13 +315,13 @@
   </si>
   <si>
     <t>TF13(15B11MA111)-126
-/NFMATH2</t>
+/SHP</t>
   </si>
   <si>
     <t>LH1H2(24B11EC111) -123 /BAB</t>
   </si>
   <si>
-    <t>PF5F6F16(18B15GE111)/EDD/CADD03/RAK/HAB/PSH</t>
+    <t>PF5F6F18(18B15GE111)/EDD/CADD03/RAK/HAB/PSH</t>
   </si>
   <si>
     <t>PF7F8F17(18B15GE111)/EDD/CADD03//NIK/SUM/PRJ/RAVI</t>
@@ -345,13 +339,13 @@
     <t>TE1(15B11PH111)-121/NFPHY1</t>
   </si>
   <si>
-    <t>PF3(15B1HS112) -246/HIMANSHI</t>
+    <t>PF3(15B1HS112) -246/DEV</t>
   </si>
   <si>
     <t>PF7(15B1HS112)-240/ANB</t>
   </si>
   <si>
-    <t>PF21F22F24(24B15CS111)-/CL1/ARJ/NIB/NFCS1</t>
+    <t>PF21F22(24B15CS111)-/CL1/ARJ/NIB/NFCS1</t>
   </si>
   <si>
     <t>PF10(15B1HS112)- 246/AKS</t>
@@ -367,10 +361,10 @@
     <t>PF11(24B15EC111)-BE LAB-I/BHC</t>
   </si>
   <si>
-    <t>PF21(24B15EC111)-BE LAB-I/KDT</t>
-  </si>
-  <si>
-    <t>PF1F2F3(24B15CS111)-CL1/ANKIT/SHM/VIS</t>
+    <t>PF21(24B15EC111)-BE LAB-II/KDT</t>
+  </si>
+  <si>
+    <t>PF1F2F3(24B15CS111)-CL1/ANKIT/SHM/VIS/DEEPTI</t>
   </si>
   <si>
     <t>PF12(24B15EC111)-DE LAB/MAG</t>
@@ -379,13 +373,13 @@
     <t>PF17(24B15EC111)-DE LAB/ABK</t>
   </si>
   <si>
-    <t>PF5(24B15EC111)-BE LAB-II/SIS</t>
-  </si>
-  <si>
-    <t>TE1(24B11EC111)-116/JMN</t>
-  </si>
-  <si>
-    <t>PF4(15B1HS112)-240/MEENAKSHI</t>
+    <t>PF5(24B15EC111)-BE LAB-II/AJK</t>
+  </si>
+  <si>
+    <t>TE1(24B11EC111)-116//PRK</t>
+  </si>
+  <si>
+    <t>PF4(15B1HS112)-240/NIC</t>
   </si>
   <si>
     <t>LH3H4(15B11CI1111) -SR05 
@@ -395,7 +389,7 @@
     <t>PE4(15B1HS112)-240/DEV</t>
   </si>
   <si>
-    <t>PF6(15B1HS112)/240/MEENAKSHI</t>
+    <t>PF6(15B1HS112)/240/EKS</t>
   </si>
   <si>
     <t>LH1H2(15B11MA111)-117
@@ -419,7 +413,7 @@
     <t>TF14(15B11PH111)-111/NAK</t>
   </si>
   <si>
-    <t>LF7F8(15B11CI1111) - 118/HIA</t>
+    <t>LF7F8(15B11CI1111) - 118/HIB</t>
   </si>
   <si>
     <t>LF7F8(15B11MA111)-118
@@ -442,7 +436,7 @@
     <t>LF24F25(15B11PH111) -123/NFPHY2</t>
   </si>
   <si>
-    <t>LH3H4(15B11HS112) -111/EKTA</t>
+    <t>LH3H4(15B11HS112) -111/EKS</t>
   </si>
   <si>
     <t>LE3E4(15B11CI1111) - 123/TWT</t>
@@ -451,17 +445,18 @@
     <t>LH1H2(15B11CI1111) -111 /GAH</t>
   </si>
   <si>
-    <t>TF9(15B11CI1111) -126/NFCS4</t>
-  </si>
-  <si>
-    <t>TF16(15B11CI1111) -116/TKW</t>
+    <t>TF9(15B11CI1111) -126
+/RISHAB</t>
+  </si>
+  <si>
+    <t>TF18(15B11CI1111) -116/DEEPTI</t>
   </si>
   <si>
     <t>LF11F12(15B11PH111) -118
 /SKH</t>
   </si>
   <si>
-    <t>TF21(15B11PH111)-113/SKH</t>
+    <t>TF21(15B11PH111)-117/SKH</t>
   </si>
   <si>
     <t>LE3E4(15B11HS112) -123/ANB</t>
@@ -476,7 +471,7 @@
     <t>TE3(15B11CI1111) -127/TWT</t>
   </si>
   <si>
-    <t>TF16(24B11EC111)-116/RAV</t>
+    <t>TF18(24B11EC111)-116/RPV</t>
   </si>
   <si>
     <t>LF9F10(15B11PH111) -
@@ -489,13 +484,13 @@
     <t>TF3(15B11CI1111) -116/AVINASH</t>
   </si>
   <si>
-    <t>TF3(15B11PH111)-113/PKC</t>
+    <t>TF3(15B11PH111)-117/PKC</t>
   </si>
   <si>
     <t>TE2(15B11CI111) -121/KNS</t>
   </si>
   <si>
-    <t>PF25(24B15EC111) -/BE LAB -II/</t>
+    <t>PF25(24B15EC111) -/BE LAB -II/RAS</t>
   </si>
   <si>
     <t>TF4(15B11PH111)-121/URS</t>
@@ -505,7 +500,10 @@
   </si>
   <si>
     <t>LF24F25(15B11CI111) -123
-/NFCS1</t>
+/SANTOSH</t>
+  </si>
+  <si>
+    <t>TF24(15B11CI111) -126/NFCS1</t>
   </si>
   <si>
     <t>WEDNESDAY</t>
@@ -514,13 +512,13 @@
     <t>LF11F12(24B11EC111) -SR05 /RUS</t>
   </si>
   <si>
-    <t>LE1E2(24B11EC111) -123 /JMN</t>
+    <t>LE1E2(24B11EC111) -123 /PRK</t>
   </si>
   <si>
     <t>TF8(24B11EC111)-116/ATK</t>
   </si>
   <si>
-    <t>TE3(24B11EC111)-116/MEA</t>
+    <t>TE3(24B11EC111)-116/MAG</t>
   </si>
   <si>
     <t>PF7(15B17PH171)-41//BHT</t>
@@ -529,8 +527,7 @@
     <t>PH2(15B17PH171)-027/NAK/NFPHY3</t>
   </si>
   <si>
-    <t>LF13F14(15B11MA111)-117
-/NFMATHS3</t>
+    <t>LF13F14(15B11MA111)-117/SHP</t>
   </si>
   <si>
     <t>PF13(15B17PH171)/41</t>
@@ -558,16 +555,16 @@
     <t>PF17(15B1HS112)-246/EKS</t>
   </si>
   <si>
-    <t>PE1(24B15EC111) - BE LAB-I/PAA</t>
-  </si>
-  <si>
-    <t>PF4F5F6(24B15CS111)-CL1/TKW/TWT/VIS</t>
+    <t>PE1(24B15EC111) - BE LAB-II/PAA</t>
+  </si>
+  <si>
+    <t>PF4F5F6(24B15CS111)-CL1/AKB/TWT/VIS</t>
   </si>
   <si>
     <t>TF8(15B11PH111)-127/URS</t>
   </si>
   <si>
-    <t>PH2H3H4(24B15CS111)-CL1/TKW/VIS/KKL</t>
+    <t>PH2H3H4(24B15CS111)-CL1/AKB/VIS/SANTOSH</t>
   </si>
   <si>
     <t>PH4(24B15EC111) - DE LAB/AJK</t>
@@ -579,16 +576,19 @@
     <t>TF7(15B11PH111)-126/URS</t>
   </si>
   <si>
-    <t>PF22(15B1HS112)-246/DEV</t>
-  </si>
-  <si>
-    <t>PH3(15B1HS112)- 240/SANJAY</t>
+    <t>LF24F25(24B11EC111) -111/RAS</t>
+  </si>
+  <si>
+    <t>PF22(15B1HS112)-246/SHV</t>
+  </si>
+  <si>
+    <t>PH3(15B1HS112)- 240/HIM</t>
   </si>
   <si>
     <t>PF8(24B15EC111)-BE LAB-II/ANG</t>
   </si>
   <si>
-    <t>LF24F25(15B11CI111) -111/NFCS1</t>
+    <t>LF24F25(15B11CI111) -111/SANTOSH</t>
   </si>
   <si>
     <t>PF3(24B15EC111)-/BE LAB-I/VAT</t>
@@ -619,7 +619,7 @@
     <t>LF1F2(24B11EC111) -117 /BHC</t>
   </si>
   <si>
-    <t>LF5F6(24B11EC111) - 111/SVS</t>
+    <t>LF5F6(24B11EC111) - 111/PRK</t>
   </si>
   <si>
     <t>LF1F2(15B11CI1111) -117 /VIS</t>
@@ -631,11 +631,11 @@
     <t>LE3E4(15B11PH111) -SR05/SHALU</t>
   </si>
   <si>
-    <t>PF1(15B1HS112)-/AKS</t>
+    <t>PF1(15B1HS112)-240/AKS</t>
   </si>
   <si>
     <t>LE1E2(15B11MA111)-111
-/NFMATHS4</t>
+/SHP</t>
   </si>
   <si>
     <t>LF1F2(15B11MA111)-117
@@ -645,8 +645,8 @@
     <t>LF5F6(15B11PH111) -111/ADV</t>
   </si>
   <si>
-    <t>LF16F17(15B11MA111)-118
-/NFMATHS4</t>
+    <t>LF18F17(15B11MA111)-118
+/ASP</t>
   </si>
   <si>
     <t>TF9(15B11MA111)-116
@@ -661,13 +661,13 @@
   </si>
   <si>
     <t>LE3E4(15B11MA111)-123
-/NFMATHS3</t>
+/ASP</t>
   </si>
   <si>
     <t>LF13F14(15B11CI1111) -118 /ANK</t>
   </si>
   <si>
-    <t>LE3E4(24B11EC111) -123 /MAG</t>
+    <t>LE3E4(24B11EC111) -123 /MEA</t>
   </si>
   <si>
     <t>LF21F22(24B11EC111) -SR05 
@@ -678,7 +678,7 @@
 /PKS</t>
   </si>
   <si>
-    <t>LF16F17(24B11EC111) - 
+    <t>LF18F17(24B11EC111) - 
 SR05/RPV</t>
   </si>
   <si>
@@ -692,7 +692,7 @@
   </si>
   <si>
     <t>LF24F25(15B11HS112) -123
-/MEENAKSHI</t>
+/ANB</t>
   </si>
   <si>
     <t>LF21F22(15B11CI1111) -118 
@@ -719,36 +719,39 @@
     <t>TE1(15B11MA111)-116/PKR</t>
   </si>
   <si>
-    <t>TF21(15B11CI1111) -127/SAP</t>
-  </si>
-  <si>
-    <t>TE4(15B11MA111)-121
-/NFMATH2</t>
-  </si>
-  <si>
     <t>TE2(15B11MA111)-121
 /PKR</t>
   </si>
   <si>
-    <t>TF25(15B11CI111) -116/NFCS1</t>
+    <t>TF21(15B11CI1111) -127/SAP</t>
+  </si>
+  <si>
+    <t>TE4(15B11MA111)-121
+/ASP</t>
+  </si>
+  <si>
+    <t>TF25(15B11CI111) -116/JYOTI</t>
   </si>
   <si>
     <t>TF10(15B11PH111)-126/ANK</t>
   </si>
   <si>
+    <t>TH1(15B11MA111)-111/PKS</t>
+  </si>
+  <si>
     <t>THURSDAY</t>
   </si>
   <si>
-    <t>LF5F6(24B11EC111) -SR05 /SVS</t>
+    <t>LF5F6(24B11EC111) -SR05 /PRK</t>
   </si>
   <si>
     <t>TF12(15B11CI1111) -116/ARJ</t>
   </si>
   <si>
-    <t>TF1(24B11EC111)-116/BHC</t>
-  </si>
-  <si>
-    <t>TF6(24B11EC111)-116/SVS</t>
+    <t>TF1(15B11MA111)-116/KKS</t>
+  </si>
+  <si>
+    <t>TF6(24B11EC111)-116/PRK</t>
   </si>
   <si>
     <t>TE4(24B11EC111)-116/MEA</t>
@@ -792,20 +795,19 @@
     <t>PF5(15B17PH171)-027//BHARTI/SKH</t>
   </si>
   <si>
-    <t>PE2(15B1HS112)-246/NIC</t>
+    <t>PE2(15B1HS112)-246//DEV</t>
   </si>
   <si>
     <t>PH4(15B17PH171)-027//BHARTI/NFPHY3</t>
   </si>
   <si>
-    <t>TF17(15B11MA111)-116/NFMATHS4</t>
-  </si>
-  <si>
-    <t>PE3(15B1HS112)-246/DEV</t>
-  </si>
-  <si>
-    <t>TF25(15B11MA111)-121
-/NFMATHS1</t>
+    <t>TF17(15B11MA111)-116/SHP</t>
+  </si>
+  <si>
+    <t>PE3(15B1HS112)-246/AKS</t>
+  </si>
+  <si>
+    <t>TF25(15B11MA111)-121/ASP</t>
   </si>
   <si>
     <t>PF13F14H3(18B15GE111) -EDD/CADD03/PSH/RAK/HAB</t>
@@ -828,13 +830,13 @@
     <t>TE3(15B11PH111)-121/NFPHY2</t>
   </si>
   <si>
-    <t>PF13F14H1(24B15CS111)--CL1/TWT/HIA/KKL</t>
-  </si>
-  <si>
-    <t>TF16(15B11PH111)-126/BHARTI</t>
-  </si>
-  <si>
-    <t>PE4F16F17(24B15CS111)-CL1/ANKIT/SHM/TWT</t>
+    <t>PF13F14H1(24B15CS111)--CL1/TWT/HIB/SANTOSH</t>
+  </si>
+  <si>
+    <t>TF18(15B11PH111)-126/BHARTI</t>
+  </si>
+  <si>
+    <t>PE4F18F17(24B15CS111)-CL1/ANKIT/SHM/TWT</t>
   </si>
   <si>
     <t>LF21F22(15B11CI1111) -148 /SAP</t>
@@ -847,20 +849,17 @@
     <t>LF21F22(15B11PH111) -117/VM</t>
   </si>
   <si>
-    <t>TF1(15B11MA111)-126/KKS</t>
-  </si>
-  <si>
     <t>PF22(24B15EC111)-/DE LAB/KDT</t>
   </si>
   <si>
-    <t>PF16(24B15EC111)/BE LAB-I/ABK</t>
-  </si>
-  <si>
-    <t>LF16F17(15B11CI1111) -111 
-/TKW</t>
-  </si>
-  <si>
-    <t>TF12(15B11MA111)-127/NFMATHS3</t>
+    <t>PF18(24B15EC111)/BE LAB-II/ABK</t>
+  </si>
+  <si>
+    <t>LF18F17(15B11CI1111) -111 
+/MOHIT</t>
+  </si>
+  <si>
+    <t>TF12(15B11MA111)-127/SHP</t>
   </si>
   <si>
     <t>PH1(24B15EC111)-BE LAB-I/PAA</t>
@@ -870,7 +869,7 @@
 /PKR</t>
   </si>
   <si>
-    <t>TF21(15B11MA111)-113/NFMATHS4</t>
+    <t>TF21(15B11MA111)-117/ASP</t>
   </si>
   <si>
     <t>LF3F4(24B11EC111) -117 /RUS</t>
@@ -889,10 +888,10 @@
     <t>TF17(15B11PH111)-111/BHARTI</t>
   </si>
   <si>
-    <t>LF9F10(15B11CI1111) -123 /NFCS4</t>
-  </si>
-  <si>
-    <t>LE1E2(15B11CI1111) -123/NFCS5</t>
+    <t>LF9F10(15B11CI1111) -123 /JYOTI</t>
+  </si>
+  <si>
+    <t>LE1E2(15B11CI1111) -123/RISHAB</t>
   </si>
   <si>
     <t>LF13F14(15B11HS112) -111
@@ -926,22 +925,19 @@
     <t>TF2(15B11CI1111) -121/VIS</t>
   </si>
   <si>
-    <t>TF17(15B11CI1111) -121/TKW</t>
-  </si>
-  <si>
-    <t>PH3(24B15EC111)/DE LAB/ABK</t>
+    <t>TF17(15B11CI1111) -121/DEEPTI</t>
+  </si>
+  <si>
+    <t>PH3(24B15EC111)/BE LAB II/ABK</t>
   </si>
   <si>
     <t>TH2(15B11PH111)-116/SKA</t>
   </si>
   <si>
-    <t>TF24(15B11CI111) -116/NFCS1</t>
-  </si>
-  <si>
     <t>TF7(15B11MA111)-126 /MSZ</t>
   </si>
   <si>
-    <t>TF12(15B11PH111)-113/SKH</t>
+    <t>TF12(15B11PH111)-116/SKH</t>
   </si>
   <si>
     <t>TF9(15B11PH111)-118/ANK</t>
@@ -956,17 +952,25 @@
     <t>TF3(15B11MA111)-SR05/NEA</t>
   </si>
   <si>
+    <t>PF25(24B15CS111)-CL4/SANTOSH</t>
+  </si>
+  <si>
+    <t>TF1(24B11EC111)-123/BHC</t>
+  </si>
+  <si>
     <t>FRIDAY</t>
   </si>
   <si>
-    <t>TF22(15B11MA111)-116/NFMATHS4</t>
+    <t>TF22(15B11MA111)-116/ASP</t>
+  </si>
+  <si>
+    <t>TF2(24B11EC111-121/BHC</t>
   </si>
   <si>
     <t>TF14(24B11EC111)-116/ATK</t>
   </si>
   <si>
-    <t>LE3E4(15B11MA111)-148
-/NFMATHS</t>
+    <t>LE3E4(15B11MA111)-148/ASP</t>
   </si>
   <si>
     <t>LF11F12(15B11HS112) -123/DEV</t>
@@ -976,7 +980,7 @@
 /ATK</t>
   </si>
   <si>
-    <t>LF7F8(15B11CI1111) - 148/HIA</t>
+    <t>LF7F8(15B11CI1111) - 148/HIB</t>
   </si>
   <si>
     <t>LF7F8(15B11PH111) -148/URS</t>
@@ -991,10 +995,7 @@
     <t>PF22(15B17PH171)-41//AMV/ANK</t>
   </si>
   <si>
-    <t>LF16F17(15B11CI1111) -111 /TKW</t>
-  </si>
-  <si>
-    <t>PF16(15B17PH171)-027//ANK/SKA</t>
+    <t>PF18(15B17PH171)-027//ANK/SKA</t>
   </si>
   <si>
     <t>LF24F25(15B11PH111) -123
@@ -1018,7 +1019,7 @@
     <t>PF13(24B15EC111)-BE LAB-I/NIY</t>
   </si>
   <si>
-    <t>LF16F17(24B11EC111) -117 /RPV</t>
+    <t>LF18F17(24B11EC111) -117 /RPV</t>
   </si>
   <si>
     <t>LH1H2(24B11EC111) -SR05 
@@ -1028,6 +1029,9 @@
     <t>PE1E2E3(24B15CS111)-CL1/ARJ/SHM/TKW/NFCS1</t>
   </si>
   <si>
+    <t>TF12(24B11EC111)-126/RUS</t>
+  </si>
+  <si>
     <t>PF14(24B15EC111)-DE LAB/VKM</t>
   </si>
   <si>
@@ -1035,29 +1039,25 @@
 /KUM</t>
   </si>
   <si>
-    <t>TF2(24B11EC111)-116/BHC</t>
+    <t>TF2(15B11MA111))-116/KKS</t>
   </si>
   <si>
     <t>PF11(15B1HS112)-246/NIC</t>
   </si>
   <si>
-    <t>LF1F2(15B11CI1111) -123/VIS</t>
+    <t>LF1F2(24B11EC111) -123/BHC</t>
   </si>
   <si>
     <t>LH1H2(15B11CI1111) - SR05/GAH</t>
   </si>
   <si>
-    <t>PE2(24B15EC111) -/BE LAB-I/JMN</t>
-  </si>
-  <si>
-    <t>TF21(24B11EC111)-121/RAV</t>
+    <t>PE2(24B15EC111) -/BE LAB-II/AJK</t>
+  </si>
+  <si>
+    <t>TF21(24B11EC111)-121/RPV</t>
   </si>
   <si>
     <t>PF12(15B1HS112)/-240/DEV</t>
-  </si>
-  <si>
-    <t>LF16F17(15B11MA111)-117
-/NFMATHS4</t>
   </si>
   <si>
     <t>LF3F4(15B11MA111)-111
@@ -1067,6 +1067,10 @@
     <t>LF3F4(15B11CI1111) - 111/AKB</t>
   </si>
   <si>
+    <t>LF13F14(15B11MA111)-117
+/SHP</t>
+  </si>
+  <si>
     <t>TF1(15B11PH111)-126/AMV</t>
   </si>
   <si>
@@ -1080,7 +1084,7 @@
     <t>LF3F4(24B11EC111) -111 /RUS</t>
   </si>
   <si>
-    <t>LF9F10(15B11CI1111) -118 /NFCS4</t>
+    <t>LF9F10(15B11CI1111) -118 /JYOTI</t>
   </si>
   <si>
     <t>LH3H4(15B11MA111)-148
@@ -1090,10 +1094,16 @@
     <t>LF3F4(15B11HS112) -111/EKS</t>
   </si>
   <si>
+    <t>LE3E4(15B11CI1111) -SR05 /TWT</t>
+  </si>
+  <si>
     <t>LH3H4(24B11EC111) -111 
 /BAB</t>
   </si>
   <si>
+    <t>TF6(15B11PH111)-121/URS</t>
+  </si>
+  <si>
     <t>TH4(24B11EC111) -116/BAB</t>
   </si>
   <si>
@@ -1125,28 +1135,22 @@
     <t>LF21F22(15B11PH111) -123/VM</t>
   </si>
   <si>
-    <t>TF12(24B11EC111)-126/RUS</t>
-  </si>
-  <si>
-    <t>PF24(15B1HS112)-246/MEENAKSHI</t>
+    <t>PF24(15B1HS112)-246/MEENAKSHI/ANSHIKA</t>
   </si>
   <si>
     <t>LF1F2(15B11PH111) -SR05/AMV</t>
   </si>
   <si>
-    <t>TF2(15B11MA111)-127/KKS</t>
-  </si>
-  <si>
-    <t>PF25(15B1HS112)-240/HIMANSHI</t>
+    <t>PF25(15B17PH171)-027/NFPHY2</t>
+  </si>
+  <si>
+    <t>PF25(15B1HS112)-240/HIMANSHI/RACHNA</t>
   </si>
   <si>
     <t>TF13(15B11PH111)-121/NAK</t>
   </si>
   <si>
-    <t>PF25(15B17PH171)-027/NFPHY2</t>
-  </si>
-  <si>
-    <t>PF24(24B15CS111)-CL1/NFCS1</t>
+    <t>PF24(24B15CS111) - /CL1//RISHAB NEGI</t>
   </si>
   <si>
     <t>SATURDAY</t>
@@ -1176,20 +1180,21 @@
     <t>LH1H2(15B11PH111) -3029/SKA</t>
   </si>
   <si>
-    <t>LF5F6(24B11EC111) -118 /SVS</t>
-  </si>
-  <si>
-    <t>PE4(24B15EC111)/BE LAB-I/DKA</t>
+    <t>LF5F6(24B11EC111) -118 
+/PRK</t>
+  </si>
+  <si>
+    <t>PE4(24B15EC111)/BE LAB-II/DKA</t>
   </si>
   <si>
     <t>LF13F14(15B11CI1111)-3023 
 /ANKIT</t>
   </si>
   <si>
-    <t>LF1F2(24B11EC111) - 3040/BHC</t>
-  </si>
-  <si>
-    <t>LH1H2(15B11CI1111) -3029
+    <t>LF1F2(24B11CI111) - 3040/VIS</t>
+  </si>
+  <si>
+    <t>LH1H2(15B11CI1111) -3028
 /GAH</t>
   </si>
   <si>
@@ -1201,18 +1206,18 @@
   </si>
   <si>
     <t>LE3E4(15B11MA111)-SR05
-/NFMATH3</t>
+/ASP</t>
   </si>
   <si>
     <t>LH3H4(15B11CI1111)-123 
 /NIB</t>
   </si>
   <si>
-    <t>LF16F17(15B11PH111) -
+    <t>LF18F17(15B11PH111) -
 SR05/BHT</t>
   </si>
   <si>
-    <t>LE1E2(15B11CI1111) -111 /NFCS5</t>
+    <t>LE1E2(15B11CI1111) -111 /RISHAB</t>
   </si>
   <si>
     <t>LF21F22(24B11EC111) -117 /RPV</t>
@@ -1222,27 +1227,24 @@
 /SAP</t>
   </si>
   <si>
-    <t>LE1E2(24B11EC111) -111 /JMN</t>
-  </si>
-  <si>
-    <t>LE3E4(15B11CI1111) -SR05 /TWT</t>
+    <t>LE1E2(24B11EC111) -111 /PRK</t>
   </si>
   <si>
     <t>LH3H4(24B11EC111) -123 /BAB</t>
   </si>
   <si>
     <t>LE3E4(24B11EC111) -SR05 
-/MAG</t>
+/MEA</t>
   </si>
   <si>
     <t>TF14(15B11MA111)-121
 /PKR</t>
   </si>
   <si>
-    <t>LF16F17(15B11HS112) -148//DEV</t>
-  </si>
-  <si>
-    <t>LF9F10(15B11CI1111) -138 /NFCS4</t>
+    <t>LF18F17(15B11HS112) -148//DEV</t>
+  </si>
+  <si>
+    <t>LF9F10(15B11CI1111) -138 /JYOTI</t>
   </si>
   <si>
     <t>LF9F10(24B11EC111) -138 
@@ -1250,7 +1252,7 @@
   </si>
   <si>
     <t>TE3(15B11MA111)-126
-/NFMATH4</t>
+/ASP</t>
   </si>
   <si>
     <t>TF4(15B11MA111)-116/PKS</t>
@@ -1271,7 +1273,7 @@
     <t>LF1F2(15B11PH111) -3040/AMV</t>
   </si>
   <si>
-    <t>TF16(15B11MA111)-113/PKS</t>
+    <t>TF18(15B11MA111)-113/PKS</t>
   </si>
   <si>
     <t>PF24(18B15GE111)/EDD/CADD03/RAK</t>
@@ -1433,7 +1435,7 @@
     <t>Deepak Verma</t>
   </si>
   <si>
-    <t>Software Development Fundamentals Lab-I</t>
+    <t>Software Development Fundamentals</t>
   </si>
   <si>
     <t>24B15CS111</t>
@@ -1796,7 +1798,7 @@
     <t>PAA</t>
   </si>
   <si>
-    <t>PKRul Arora</t>
+    <t>Parul Arora</t>
   </si>
   <si>
     <t>26</t>
@@ -1832,10 +1834,10 @@
     <t>28</t>
   </si>
   <si>
-    <t>HIA</t>
-  </si>
-  <si>
-    <t>Himanshu Agrawal</t>
+    <t>HIB</t>
+  </si>
+  <si>
+    <t>Himani Bansal</t>
   </si>
   <si>
     <t>57</t>
@@ -1850,19 +1852,31 @@
     <t>29</t>
   </si>
   <si>
+    <t>ASP</t>
+  </si>
+  <si>
+    <t>Asim Patra</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>GAH</t>
+  </si>
+  <si>
+    <t>Gaurav Sinha</t>
+  </si>
+  <si>
+    <t>SHP</t>
+  </si>
+  <si>
+    <t>Shivani Pant</t>
+  </si>
+  <si>
     <t>VIS</t>
   </si>
   <si>
     <t>Vikas Sharma</t>
-  </si>
-  <si>
-    <t>58</t>
-  </si>
-  <si>
-    <t>GAH</t>
-  </si>
-  <si>
-    <t>Gaurav Sinha</t>
   </si>
 </sst>
 </file>
@@ -2117,15 +2131,15 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.29"/>
-    <col customWidth="1" min="2" max="2" width="48.57"/>
-    <col customWidth="1" min="3" max="3" width="33.57"/>
-    <col customWidth="1" min="4" max="4" width="66.0"/>
-    <col customWidth="1" min="5" max="5" width="50.57"/>
-    <col customWidth="1" min="6" max="6" width="42.71"/>
-    <col customWidth="1" min="7" max="7" width="51.71"/>
-    <col customWidth="1" min="8" max="8" width="57.29"/>
-    <col customWidth="1" min="9" max="9" width="49.43"/>
+    <col customWidth="1" min="1" max="1" width="31.43"/>
+    <col customWidth="1" min="2" max="2" width="53.14"/>
+    <col customWidth="1" min="3" max="3" width="42.0"/>
+    <col customWidth="1" min="4" max="4" width="41.43"/>
+    <col customWidth="1" min="5" max="5" width="41.14"/>
+    <col customWidth="1" min="6" max="6" width="52.14"/>
+    <col customWidth="1" min="7" max="7" width="62.0"/>
+    <col customWidth="1" min="8" max="8" width="54.43"/>
+    <col customWidth="1" min="9" max="9" width="89.86"/>
     <col customWidth="1" min="10" max="26" width="8.71"/>
   </cols>
   <sheetData>
@@ -2169,591 +2183,592 @@
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="18">
       <c r="C18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="G22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="C23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="H23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="B24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="D25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="B26" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="B27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="B28" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="B29" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="B30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="B31" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="B32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="B33" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="B34" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="B35" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="B36" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="B37" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="B38" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E38" s="1" t="s">
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="D39" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1"/>
+    </row>
     <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="D42" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="B43" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="B44" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="B45" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="B46" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2867,7 +2882,7 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="B53" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>210</v>
@@ -2903,17 +2918,17 @@
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
+      <c r="C55" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="D55" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="C56" s="1" t="s">
-        <v>222</v>
-      </c>
       <c r="D56" s="1" t="s">
         <v>223</v>
       </c>
@@ -2921,136 +2936,137 @@
         <v>224</v>
       </c>
     </row>
-    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="G57" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
     <row r="58" ht="15.75" customHeight="1"/>
     <row r="59" ht="15.75" customHeight="1"/>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="D61" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="B62" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="B63" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="B64" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="B65" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="B66" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="B67" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H67" s="1" t="s">
         <v>260</v>
       </c>
     </row>
@@ -3151,1100 +3167,1130 @@
       <c r="B74" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="G74" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="G74" s="1" t="s">
+      <c r="H74" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="H74" s="1" t="s">
+    </row>
+    <row r="75" ht="15.75" customHeight="1">
+      <c r="B75" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="75" ht="15.75" customHeight="1">
-      <c r="C75" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="H75" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="H75" s="1" t="s">
+    </row>
+    <row r="76" ht="15.75" customHeight="1">
+      <c r="B76" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="76" ht="15.75" customHeight="1"/>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1"/>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="C79" s="1" t="s">
+      <c r="A79" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="G79" s="1" t="s">
+    </row>
+    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1">
+      <c r="C81" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="I79" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="80" ht="15.75" customHeight="1">
-      <c r="B80" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D80" s="1" t="s">
+      <c r="G81" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="I81" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="H80" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="81" ht="15.75" customHeight="1">
-      <c r="B81" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="I81" s="1" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="B82" s="1" t="s">
-        <v>309</v>
+        <v>28</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>301</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>312</v>
+        <v>303</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="B83" s="1" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>123</v>
+        <v>263</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>316</v>
+        <v>308</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="B84" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>167</v>
+        <v>310</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="B85" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>323</v>
+        <v>315</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>324</v>
+        <v>121</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>325</v>
+        <v>317</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="B86" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>328</v>
+        <v>166</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>162</v>
+        <v>320</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="H86" s="1" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="B87" s="1" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>335</v>
+        <v>325</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>326</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>44</v>
+        <v>327</v>
       </c>
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="B88" s="1" t="s">
-        <v>337</v>
+        <v>32</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>340</v>
+        <v>330</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>331</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="B89" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="90" ht="15.75" customHeight="1">
+      <c r="B90" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="E90" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="G90" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="G89" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H89" s="1" t="s">
+      <c r="H90" s="1" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
-      <c r="C90" s="1" t="s">
+    <row r="91" ht="15.75" customHeight="1">
+      <c r="B91" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="G90" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H90" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="91" ht="15.75" customHeight="1">
-      <c r="C91" s="1" t="s">
+      <c r="G91" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H91" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D91" s="1" t="s">
+    </row>
+    <row r="92" ht="15.75" customHeight="1">
+      <c r="D92" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="G91" s="1" t="s">
+      <c r="G92" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H92" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="92" ht="15.75" customHeight="1">
-      <c r="B92" s="1" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="B93" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="94" ht="15.75" customHeight="1"/>
+      <c r="G93" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="94" ht="15.75" customHeight="1">
+      <c r="B94" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
     <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="97" ht="15.75" customHeight="1">
-      <c r="C97" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="D97" s="1" t="s">
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1">
+      <c r="A100" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="E97" s="1" t="s">
+    </row>
+    <row r="101" ht="15.75" customHeight="1">
+      <c r="C101" s="1" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="98" ht="15.75" customHeight="1">
-      <c r="B98" s="1" t="s">
+      <c r="D101" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="E101" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="99" ht="15.75" customHeight="1">
-      <c r="B99" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="100" ht="15.75" customHeight="1">
-      <c r="B100" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="101" ht="15.75" customHeight="1">
-      <c r="B101" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="B102" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="B103" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="B104" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>379</v>
+        <v>166</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="B105" s="1" t="s">
-        <v>381</v>
+        <v>260</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>383</v>
+        <v>196</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="B106" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="107" ht="15.75" customHeight="1">
+      <c r="B107" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="108" ht="15.75" customHeight="1">
+      <c r="B108" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="109" ht="15.75" customHeight="1">
+      <c r="B109" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="E109" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C106" s="1" t="s">
+    </row>
+    <row r="110" ht="15.75" customHeight="1">
+      <c r="B110" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="C110" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="E106" s="1" t="s">
+      <c r="D110" s="1" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="107" ht="15.75" customHeight="1">
-      <c r="D107" s="1" t="s">
+      <c r="E110" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="E107" s="1" t="s">
+    </row>
+    <row r="111" ht="15.75" customHeight="1">
+      <c r="D111" s="1" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="108" ht="15.75" customHeight="1">
-      <c r="D108" s="1" t="s">
+      <c r="E111" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="E108" s="1" t="s">
+    </row>
+    <row r="112" ht="15.75" customHeight="1">
+      <c r="D112" s="1" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="109" ht="15.75" customHeight="1">
-      <c r="C109" s="1" t="s">
+      <c r="E112" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="110" ht="15.75" customHeight="1">
-      <c r="C110" s="1" t="s">
+    <row r="113" ht="15.75" customHeight="1">
+      <c r="C113" s="1" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1">
-      <c r="B113" s="1" t="s">
+    <row r="114" ht="15.75" customHeight="1">
+      <c r="C114" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="G113" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="H113" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="I113" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="114" ht="15.75" customHeight="1">
-      <c r="B114" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="G114" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="H114" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="I114" s="1" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="115" ht="15.75" customHeight="1">
-      <c r="B115" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="H115" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="I115" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="116" ht="15.75" customHeight="1">
-      <c r="B116" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="G116" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="H116" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="I116" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
+    </row>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
     <row r="117" ht="15.75" customHeight="1">
       <c r="B117" s="1" t="s">
-        <v>424</v>
+        <v>396</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>425</v>
+        <v>397</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>426</v>
+        <v>398</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>427</v>
+        <v>396</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>428</v>
+        <v>397</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>429</v>
+        <v>398</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>430</v>
+        <v>399</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>431</v>
+        <v>400</v>
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
       <c r="B118" s="1" t="s">
-        <v>432</v>
+        <v>401</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>433</v>
+        <v>402</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>434</v>
+        <v>403</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>435</v>
+        <v>404</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>436</v>
+        <v>405</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>437</v>
+        <v>406</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>438</v>
+        <v>407</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>439</v>
+        <v>408</v>
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
       <c r="B119" s="1" t="s">
-        <v>440</v>
+        <v>409</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>441</v>
+        <v>410</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>442</v>
+        <v>411</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>443</v>
+        <v>412</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>444</v>
+        <v>413</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>445</v>
+        <v>414</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>446</v>
+        <v>415</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>447</v>
+        <v>416</v>
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1">
       <c r="B120" s="1" t="s">
-        <v>448</v>
+        <v>417</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>449</v>
+        <v>418</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>450</v>
+        <v>419</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>451</v>
+        <v>420</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>452</v>
+        <v>421</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>453</v>
+        <v>422</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>454</v>
+        <v>423</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>455</v>
+        <v>424</v>
       </c>
     </row>
     <row r="121" ht="15.75" customHeight="1">
       <c r="B121" s="1" t="s">
-        <v>456</v>
+        <v>425</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>457</v>
+        <v>426</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>458</v>
+        <v>427</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>459</v>
+        <v>428</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>460</v>
+        <v>429</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>461</v>
+        <v>430</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>462</v>
+        <v>431</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>463</v>
+        <v>432</v>
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1">
       <c r="B122" s="1" t="s">
-        <v>464</v>
+        <v>433</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>465</v>
+        <v>434</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>466</v>
+        <v>435</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>468</v>
+        <v>437</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>469</v>
+        <v>438</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>470</v>
+        <v>439</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>471</v>
+        <v>440</v>
       </c>
     </row>
     <row r="123" ht="15.75" customHeight="1">
       <c r="B123" s="1" t="s">
-        <v>472</v>
+        <v>441</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>473</v>
+        <v>442</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>474</v>
+        <v>443</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>475</v>
+        <v>444</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>476</v>
+        <v>445</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>477</v>
+        <v>446</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="124" ht="15.75" customHeight="1">
       <c r="B124" s="1" t="s">
-        <v>478</v>
+        <v>449</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>479</v>
+        <v>450</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>480</v>
+        <v>451</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>481</v>
+        <v>452</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>482</v>
+        <v>453</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>483</v>
+        <v>454</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="I124" s="1" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="125" ht="15.75" customHeight="1">
       <c r="B125" s="1" t="s">
-        <v>484</v>
+        <v>457</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>485</v>
+        <v>458</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>486</v>
+        <v>459</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>488</v>
+        <v>461</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>489</v>
+        <v>462</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1">
       <c r="B126" s="1" t="s">
-        <v>490</v>
+        <v>465</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>491</v>
+        <v>466</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>492</v>
+        <v>467</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>493</v>
+        <v>468</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>494</v>
+        <v>469</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>495</v>
+        <v>470</v>
+      </c>
+      <c r="H126" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
       <c r="B127" s="1" t="s">
-        <v>496</v>
+        <v>473</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>497</v>
+        <v>474</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>498</v>
+        <v>475</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>499</v>
+        <v>476</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>500</v>
+        <v>477</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>501</v>
+        <v>478</v>
       </c>
     </row>
     <row r="128" ht="15.75" customHeight="1">
       <c r="B128" s="1" t="s">
-        <v>502</v>
+        <v>479</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>503</v>
+        <v>480</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>504</v>
+        <v>481</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>505</v>
+        <v>482</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>506</v>
+        <v>483</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>507</v>
+        <v>484</v>
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
       <c r="B129" s="1" t="s">
-        <v>508</v>
+        <v>485</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>509</v>
+        <v>486</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>510</v>
+        <v>487</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>511</v>
+        <v>488</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>512</v>
+        <v>489</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>513</v>
+        <v>490</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
       <c r="B130" s="1" t="s">
-        <v>514</v>
+        <v>491</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>515</v>
+        <v>492</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>516</v>
+        <v>493</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>517</v>
+        <v>494</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>518</v>
+        <v>495</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>519</v>
+        <v>496</v>
       </c>
     </row>
     <row r="131" ht="15.75" customHeight="1">
       <c r="B131" s="1" t="s">
-        <v>520</v>
+        <v>497</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>521</v>
+        <v>498</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>522</v>
+        <v>499</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>523</v>
+        <v>500</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>524</v>
+        <v>501</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>525</v>
+        <v>502</v>
       </c>
     </row>
     <row r="132" ht="15.75" customHeight="1">
       <c r="B132" s="1" t="s">
-        <v>526</v>
+        <v>503</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>527</v>
+        <v>504</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>528</v>
+        <v>505</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>529</v>
+        <v>506</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>530</v>
+        <v>507</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>531</v>
+        <v>508</v>
       </c>
     </row>
     <row r="133" ht="15.75" customHeight="1">
       <c r="B133" s="1" t="s">
-        <v>532</v>
+        <v>509</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>533</v>
+        <v>510</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>534</v>
+        <v>511</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>535</v>
+        <v>512</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>536</v>
+        <v>513</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>537</v>
+        <v>514</v>
       </c>
     </row>
     <row r="134" ht="15.75" customHeight="1">
       <c r="B134" s="1" t="s">
-        <v>538</v>
+        <v>515</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>539</v>
+        <v>516</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>540</v>
+        <v>517</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>542</v>
+        <v>519</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>543</v>
+        <v>520</v>
       </c>
     </row>
     <row r="135" ht="15.75" customHeight="1">
       <c r="B135" s="1" t="s">
-        <v>544</v>
+        <v>521</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>545</v>
+        <v>522</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>546</v>
+        <v>523</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>547</v>
+        <v>524</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>548</v>
+        <v>525</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>549</v>
+        <v>526</v>
       </c>
     </row>
     <row r="136" ht="15.75" customHeight="1">
       <c r="B136" s="1" t="s">
-        <v>550</v>
+        <v>527</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>551</v>
+        <v>528</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>552</v>
+        <v>529</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>553</v>
+        <v>530</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>554</v>
+        <v>531</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>555</v>
+        <v>532</v>
       </c>
     </row>
     <row r="137" ht="15.75" customHeight="1">
       <c r="B137" s="1" t="s">
-        <v>556</v>
+        <v>533</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>557</v>
+        <v>534</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>558</v>
+        <v>535</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>559</v>
+        <v>536</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>560</v>
+        <v>537</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>561</v>
+        <v>538</v>
       </c>
     </row>
     <row r="138" ht="15.75" customHeight="1">
       <c r="B138" s="1" t="s">
-        <v>562</v>
+        <v>539</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>563</v>
+        <v>540</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>564</v>
+        <v>541</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>565</v>
+        <v>542</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>566</v>
+        <v>543</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>567</v>
+        <v>544</v>
       </c>
     </row>
     <row r="139" ht="15.75" customHeight="1">
       <c r="B139" s="1" t="s">
-        <v>568</v>
+        <v>545</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>569</v>
+        <v>546</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>570</v>
+        <v>547</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>571</v>
+        <v>548</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>572</v>
+        <v>549</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>573</v>
+        <v>550</v>
       </c>
     </row>
     <row r="140" ht="15.75" customHeight="1">
       <c r="B140" s="1" t="s">
-        <v>574</v>
+        <v>551</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>575</v>
+        <v>552</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>576</v>
+        <v>553</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>577</v>
+        <v>554</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
     </row>
     <row r="141" ht="15.75" customHeight="1">
       <c r="B141" s="1" t="s">
-        <v>578</v>
+        <v>557</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>579</v>
+        <v>558</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>580</v>
+        <v>559</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>581</v>
+        <v>560</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>582</v>
+        <v>561</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>583</v>
+        <v>562</v>
       </c>
     </row>
     <row r="142" ht="15.75" customHeight="1">
       <c r="B142" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="143" ht="15.75" customHeight="1">
+      <c r="B143" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="144" ht="15.75" customHeight="1">
+      <c r="B144" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="145" ht="15.75" customHeight="1">
+      <c r="B145" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="G145" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="C142" s="1" t="s">
+    </row>
+    <row r="146" ht="15.75" customHeight="1">
+      <c r="B146" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="D142" s="1" t="s">
+      <c r="C146" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="E142" s="1" t="s">
+      <c r="D146" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="F142" s="1" t="s">
+      <c r="E146" s="1" t="s">
         <v>588</v>
       </c>
-      <c r="G142" s="1" t="s">
+      <c r="F146" s="1" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
+      <c r="G146" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="147" ht="15.75" customHeight="1">
+      <c r="B147" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="148" ht="15.75" customHeight="1">
+      <c r="B148" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
     <row r="149" ht="15.75" customHeight="1"/>
     <row r="150" ht="15.75" customHeight="1"/>
     <row r="151" ht="15.75" customHeight="1"/>
@@ -5076,13 +5122,8 @@
     <row r="977" ht="15.75" customHeight="1"/>
     <row r="978" ht="15.75" customHeight="1"/>
     <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="121">
+  <mergeCells count="123">
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="D8:E8"/>
@@ -5106,24 +5147,26 @@
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B68:C68"/>
     <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="A60:A78"/>
+    <mergeCell ref="A79:A99"/>
+    <mergeCell ref="A100:A116"/>
+    <mergeCell ref="A117:A139"/>
+    <mergeCell ref="A140:A148"/>
     <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
     <mergeCell ref="B93:C93"/>
-    <mergeCell ref="A96:A112"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="A113:A142"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
-    <mergeCell ref="A60:A76"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B66:C66"/>
-    <mergeCell ref="A77:A95"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B76:C76"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B46:C46"/>
@@ -5153,20 +5196,20 @@
     <mergeCell ref="G66:H66"/>
     <mergeCell ref="G72:H72"/>
     <mergeCell ref="G73:H73"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="G82:I82"/>
-    <mergeCell ref="F100:I112"/>
-    <mergeCell ref="C109:E109"/>
-    <mergeCell ref="C110:E110"/>
+    <mergeCell ref="D83:E83"/>
     <mergeCell ref="G83:H83"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="G84:I84"/>
+    <mergeCell ref="C113:E113"/>
+    <mergeCell ref="C114:E114"/>
+    <mergeCell ref="E148:G148"/>
     <mergeCell ref="G85:H85"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="F96:I99"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="G87:H87"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="F100:I116"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:E12"/>

</xml_diff>

<commit_message>
chore: update 128 sem-1 tt
</commit_message>
<xml_diff>
--- a/raw/time_tables/B.Tech 128 (btech-128)/1/1.xlsx
+++ b/raw/time_tables/B.Tech 128 (btech-128)/1/1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="598">
   <si>
     <t>B.TECH. I Yr(I SEMESTER) TIMETABLE ODD SEMESTER 2025, JIIT-128</t>
   </si>
@@ -50,8 +50,7 @@
 /PKS</t>
   </si>
   <si>
-    <t>LE3E4(15B11PH111) -123
-/SHALU</t>
+    <t>LE3E4(15B11PH111) -123/URS</t>
   </si>
   <si>
     <t>LF11F12(15B11CI1111) -117/ARJ</t>
@@ -74,31 +73,31 @@
     <t>TF17(24B11EC111)-116//RPV</t>
   </si>
   <si>
-    <t>PF7F8F9(24B15CS111) - /CL1/AKB/SHG/NIB</t>
+    <t>PF7F8F9(24B15CS111) - /CL1/AKB/SHG/NIB/SAMARTH JAIN</t>
   </si>
   <si>
     <t>PF18(15B1HS112) -/240/DEV</t>
   </si>
   <si>
-    <t>PF1(24B15EC111)-/BE LAB-I/BHC</t>
+    <t>PF1(24B15EC111)-/BE LAB-I/BHC/DKA</t>
   </si>
   <si>
     <t>PF21(15B1HS112)-240/MEENAKSHI/AARUSHI</t>
   </si>
   <si>
-    <t>PF3(15B17PH171) - /41/ADV/ANK</t>
-  </si>
-  <si>
-    <t>PF17(15B17PH171)-/41 /PKC/NFPHY2</t>
-  </si>
-  <si>
-    <t>PF2(24B15EC111)-/BE LAB-II/MAG</t>
+    <t>PF3(15B17PH171) - /41/NAK</t>
+  </si>
+  <si>
+    <t>PF17(15B17PH171)-/256C /PKC</t>
+  </si>
+  <si>
+    <t>PF2(24B15EC111)-/BE LAB-II/MAG/RPV</t>
   </si>
   <si>
     <t>LF24F25(15B11MA111)-123/MSZ</t>
   </si>
   <si>
-    <t>TF24(15B11PH111)-127/SKA</t>
+    <t>TF24(15B11PH111)-127/KAS</t>
   </si>
   <si>
     <t>LH1H2(15B11PH111) -SR05/SKA</t>
@@ -107,7 +106,7 @@
     <t>LE3E4(24B11EC111)) -123/MEA</t>
   </si>
   <si>
-    <t>PE3(24B15EC111)/DE LAB/AJK</t>
+    <t>PE3(24B15EC111)/DE LAB/AJK/VAT</t>
   </si>
   <si>
     <t>LF13F14(15B11PH111) -118/NAK</t>
@@ -123,7 +122,7 @@
     <t>TF25(24B11EC111) -126/RAS</t>
   </si>
   <si>
-    <t>PF1F2F21(18B15GE111)/EDD/CADD03/PRJ/HAB/NIK</t>
+    <t>PF1F2F21(18B15GE111)/EDD/CADD03/PRJ/HAB/NIK/JUGENDRA SINGH</t>
   </si>
   <si>
     <t>LF21F22(15B11MA111)-117
@@ -134,7 +133,7 @@
 /SHP</t>
   </si>
   <si>
-    <t>PF3F4F22(18B15GE111)/EDD/CADD03/SUM/PSH/RAK/JUGENDRA SINGH</t>
+    <t>PF3F4F22(18B15GE111)/EDD/CADD03/SUM/PSH/RAK</t>
   </si>
   <si>
     <t>PF5(15B1HS112)-/240/EKS</t>
@@ -146,54 +145,55 @@
     <t>/NFMATH3</t>
   </si>
   <si>
-    <t>PE3(15B17PH171)-41/ADV/NFPHY3</t>
-  </si>
-  <si>
-    <t>PF4(15B17PH171)-/027/VM/NFPHY3</t>
-  </si>
-  <si>
-    <t>PH3(15B17PH171)- 027/SKH/SHALU</t>
+    <t>PE3(15B17PH171)-41/URS</t>
+  </si>
+  <si>
+    <t>PF4(15B17PH171)-/256C/SHALU</t>
+  </si>
+  <si>
+    <t>PH3(15B17PH171)- 41/SKA</t>
   </si>
   <si>
     <t>LF3F4(15B11CI1111) -123 /AKB</t>
   </si>
   <si>
-    <t>PF6(15B17PH171)-027/AMV/VM</t>
+    <t>PF6(15B17PH171)-256/ANK</t>
   </si>
   <si>
     <t>PE1(15B1HS112)-/246/NIC</t>
   </si>
   <si>
-    <t>PH2(24B15EC111)/BE LAB-II/ABK</t>
+    <t>PH2(24B15EC111)/BE LAB-II/ABK/ASG</t>
   </si>
   <si>
     <t>LF7F8(15B11CI1111) -111 /HIB</t>
   </si>
   <si>
-    <t>PF6(24B15EC111)/BE LAB-I/AJK</t>
+    <t>PF6(24B15EC111)/BE LAB-I/AJK/ATK</t>
   </si>
   <si>
     <t>LF9F10(15B11MA111)-118
 /NEA</t>
   </si>
   <si>
-    <t>LF9F10(15B11HS112) -118/NC</t>
+    <t>LF9F10(15B11HS112) -118
+/CHANDRESHEKHAR</t>
   </si>
   <si>
     <t>LF5F6(15B11PH111) -117/ADV</t>
   </si>
   <si>
-    <t>PF10F11F12(24B15CS111) - /CL1/ARJ/ANK/NIB</t>
-  </si>
-  <si>
-    <t>PF10(24B15EC111)/BE LAB-II/NIY</t>
+    <t>PF10F11F12(24B15CS111) - /CL1/ARJ/ANK/NIB/BAIBHAV</t>
+  </si>
+  <si>
+    <t>PF10(24B15EC111)/BE LAB-II/NIY/BKM</t>
   </si>
   <si>
     <t>LE1E2(15B11CI1111) -123 /RISHAB</t>
   </si>
   <si>
     <t>LF24F25(15B11PH111) -
-SR05/NFPHY2</t>
+SR05/NAK</t>
   </si>
   <si>
     <t>PH4(15B1HS112)-/240/AKS</t>
@@ -236,7 +236,7 @@
     <t>TE2(24B11EC111) -116/PRK</t>
   </si>
   <si>
-    <t>LH3H4(15B11PH111) -SR05/BHARTI</t>
+    <t>LH3H4(15B11PH111) -SR05/BHT</t>
   </si>
   <si>
     <t>TF22(24B11EC111)-126/RPV</t>
@@ -259,7 +259,7 @@
 /PKR</t>
   </si>
   <si>
-    <t>PF24(24B15EC111) -/DE LAB/RAS</t>
+    <t>PF24(24B15EC111) -/DE LAB/NFEC1/RUS</t>
   </si>
   <si>
     <t>LF24F25(24B11EC111) -123
@@ -288,16 +288,16 @@
 NFMATHS3</t>
   </si>
   <si>
-    <t>TF25(15B11PH111)-127/VM</t>
-  </si>
-  <si>
-    <t>PF1(15B17PH171) -41/VM/URS</t>
-  </si>
-  <si>
-    <t>PE1(15B17PH171)-41//SKA/SHALU</t>
-  </si>
-  <si>
-    <t>PF9(15B17PH171)-41/URS/NFPHY3</t>
+    <t>TF25(15B11PH111)-127/BHT</t>
+  </si>
+  <si>
+    <t>PF1(15B17PH171) -41/VM</t>
+  </si>
+  <si>
+    <t>PE1(15B17PH171)-41//SKA</t>
+  </si>
+  <si>
+    <t>PF9(15B17PH171)-41/URS</t>
   </si>
   <si>
     <t>TF24(24B11EC111) -126/RAS</t>
@@ -311,11 +311,11 @@
 /AMV</t>
   </si>
   <si>
-    <t>PF4(24B15EC111)-BE LAB-I/NIY</t>
+    <t>PF4(24B15EC111)-BE LAB-I/NIY/PRK</t>
   </si>
   <si>
     <t>TF13(15B11MA111)-126
-/SHP</t>
+/ASP</t>
   </si>
   <si>
     <t>LH1H2(24B11EC111) -123 /BAB</t>
@@ -327,16 +327,16 @@
     <t>PF7F8F17(18B15GE111)/EDD/CADD03//NIK/SUM/PRJ/RAVI</t>
   </si>
   <si>
-    <t>PF2(15B17PH171)-027/NAK/NFPHY2</t>
-  </si>
-  <si>
-    <t>PE2(15B17PH171)-027/PKC/ADV</t>
-  </si>
-  <si>
-    <t>PF10(15B17PH171)-027//NAK/PKC</t>
-  </si>
-  <si>
-    <t>TE1(15B11PH111)-121/NFPHY1</t>
+    <t>PF2(15B17PH171)-256C/BHT</t>
+  </si>
+  <si>
+    <t>PE2(15B17PH171)-256C/BHT</t>
+  </si>
+  <si>
+    <t>PF10(15B17PH171)-256C/KAS/ADV</t>
+  </si>
+  <si>
+    <t>TE1(15B11PH111)-121/SHALU</t>
   </si>
   <si>
     <t>PF3(15B1HS112) -246/DEV</t>
@@ -345,7 +345,7 @@
     <t>PF7(15B1HS112)-240/ANB</t>
   </si>
   <si>
-    <t>PF21F22(24B15CS111)-/CL1/ARJ/NIB/NFCS1</t>
+    <t>PF21F22(24B15CS111)-/CL1/ARJ/NIB/VIS</t>
   </si>
   <si>
     <t>PF10(15B1HS112)- 246/AKS</t>
@@ -358,22 +358,22 @@
 /MSZ</t>
   </si>
   <si>
-    <t>PF11(24B15EC111)-BE LAB-I/BHC</t>
-  </si>
-  <si>
-    <t>PF21(24B15EC111)-BE LAB-II/KDT</t>
-  </si>
-  <si>
-    <t>PF1F2F3(24B15CS111)-CL1/ANKIT/SHM/VIS/DEEPTI</t>
-  </si>
-  <si>
-    <t>PF12(24B15EC111)-DE LAB/MAG</t>
-  </si>
-  <si>
-    <t>PF17(24B15EC111)-DE LAB/ABK</t>
-  </si>
-  <si>
-    <t>PF5(24B15EC111)-BE LAB-II/AJK</t>
+    <t>PF11(24B15EC111)-BE LAB-I/BHC/PRK</t>
+  </si>
+  <si>
+    <t>PF21(24B15EC111)-BE LAB-II/KDT/ATK</t>
+  </si>
+  <si>
+    <t>PF1F2F3(24B15CS111)-CL1/ANKIT/BAIBHAV/SHM</t>
+  </si>
+  <si>
+    <t>PF12(24B15EC111)-DE LAB/MAG/VAT</t>
+  </si>
+  <si>
+    <t>PF17(24B15EC111)-DE LAB/ABK/RUS</t>
+  </si>
+  <si>
+    <t>PF5(24B15EC111)-BE LAB-II/AJK/MEA</t>
   </si>
   <si>
     <t>TE1(24B11EC111)-116//PRK</t>
@@ -410,7 +410,7 @@
     <t>LF11F12(15B11CI1111) -118 /ARJ</t>
   </si>
   <si>
-    <t>TF14(15B11PH111)-111/NAK</t>
+    <t>TF14(15B11PH111)-111/SHALU</t>
   </si>
   <si>
     <t>LF7F8(15B11CI1111) - 118/HIB</t>
@@ -433,7 +433,7 @@
 /NFMATHS4</t>
   </si>
   <si>
-    <t>LF24F25(15B11PH111) -123/NFPHY2</t>
+    <t>LF24F25(15B11PH111) -123/NAK</t>
   </si>
   <si>
     <t>LH3H4(15B11HS112) -111/EKS</t>
@@ -456,16 +456,13 @@
 /SKH</t>
   </si>
   <si>
-    <t>TF21(15B11PH111)-117/SKH</t>
+    <t>TF21(15B11PH111)-117/VM</t>
   </si>
   <si>
     <t>LE3E4(15B11HS112) -123/ANB</t>
   </si>
   <si>
     <t>LE1E2(15B11PH111) -111/SHALU</t>
-  </si>
-  <si>
-    <t>LE3E4(15B11PH111) -123/SHALU</t>
   </si>
   <si>
     <t>TE3(15B11CI1111) -127/TWT</t>
@@ -478,7 +475,7 @@
 SR05/ANK</t>
   </si>
   <si>
-    <t>TH1(15B11PH111)-116/ANK</t>
+    <t>TH1(15B11PH111)-116/KAS</t>
   </si>
   <si>
     <t>TF3(15B11CI1111) -116/AVINASH</t>
@@ -490,22 +487,19 @@
     <t>TE2(15B11CI111) -121/KNS</t>
   </si>
   <si>
-    <t>PF25(24B15EC111) -/BE LAB -II/RAS</t>
-  </si>
-  <si>
-    <t>TF4(15B11PH111)-121/URS</t>
-  </si>
-  <si>
-    <t>TF22(15B11PH111)-111/SKH</t>
+    <t>PF25(24B15EC111) -/BE LAB -II/NFEC1/NIY</t>
+  </si>
+  <si>
+    <t>TF4(15B11PH111)-121/PKC</t>
+  </si>
+  <si>
+    <t>TF22(15B11PH111)-111/SHALU</t>
   </si>
   <si>
     <t>LF24F25(15B11CI111) -123
 /SANTOSH</t>
   </si>
   <si>
-    <t>TF24(15B11CI111) -126/NFCS1</t>
-  </si>
-  <si>
     <t>WEDNESDAY</t>
   </si>
   <si>
@@ -521,56 +515,55 @@
     <t>TE3(24B11EC111)-116/MAG</t>
   </si>
   <si>
-    <t>PF7(15B17PH171)-41//BHT</t>
-  </si>
-  <si>
-    <t>PH2(15B17PH171)-027/NAK/NFPHY3</t>
+    <t>PF7(15B17PH171)-41/KAS/PKC</t>
+  </si>
+  <si>
+    <t>PH2(15B17PH171)-027/NAK</t>
   </si>
   <si>
     <t>LF13F14(15B11MA111)-117/SHP</t>
   </si>
   <si>
-    <t>PF13(15B17PH171)/41</t>
-  </si>
-  <si>
-    <t>TF24(15B11MA111)-121
-/NFMATHS1</t>
-  </si>
-  <si>
-    <t>PF8(15B17PH171)-027/URS/AMV</t>
-  </si>
-  <si>
-    <t>PH1(15B17PH171)-41/ANK/NFPHY2</t>
+    <t>PF13(15B17PH171)/41/ADV/PKC</t>
+  </si>
+  <si>
+    <t>TF24(15B11MA111)-121/PKS</t>
+  </si>
+  <si>
+    <t>PF8(15B17PH171)-256C/URS/AMV</t>
+  </si>
+  <si>
+    <t>PH1(15B17PH171)-41/ANK/SKH</t>
   </si>
   <si>
     <t>LF5F6(15B11CI1111) -118 /SHM</t>
   </si>
   <si>
-    <t>PF14(15B17PH171)/027</t>
-  </si>
-  <si>
-    <t>TE4(15B11PH111)-126/NFPHY2</t>
+    <t>PF14(15B17PH171)/256/SKH</t>
+  </si>
+  <si>
+    <t>TE4(15B11PH111)-126/NAK</t>
   </si>
   <si>
     <t>PF17(15B1HS112)-246/EKS</t>
   </si>
   <si>
-    <t>PE1(24B15EC111) - BE LAB-II/PAA</t>
-  </si>
-  <si>
-    <t>PF4F5F6(24B15CS111)-CL1/AKB/TWT/VIS</t>
+    <t>PE1(24B15EC111) - BE LAB-II/PAA/VKM</t>
+  </si>
+  <si>
+    <t>PF4F5F6(24B15CS111)-CL1/AKB/TWT/VIS/JATIN</t>
   </si>
   <si>
     <t>TF8(15B11PH111)-127/URS</t>
   </si>
   <si>
-    <t>PH2H3H4(24B15CS111)-CL1/AKB/VIS/SANTOSH</t>
-  </si>
-  <si>
-    <t>PH4(24B15EC111) - DE LAB/AJK</t>
-  </si>
-  <si>
-    <t>PF7(24B15EC111)-BE LAB-I/ABK</t>
+    <t>PH2H3H4(24B15CS111)-CL1/AKB/VIS/SANTOSH/SAMARTH JAIN</t>
+  </si>
+  <si>
+    <t>PH4(24B15EC111) - DE LAB/AJK/BHC</t>
+  </si>
+  <si>
+    <t>PF7(24B15EC111)-BE LAB-I/ABK/NIY</t>
   </si>
   <si>
     <t>TF7(15B11PH111)-126/URS</t>
@@ -579,19 +572,22 @@
     <t>LF24F25(24B11EC111) -111/RAS</t>
   </si>
   <si>
-    <t>PF22(15B1HS112)-246/SHV</t>
+    <t>PF22(15B1HS112)-246/RACHNA/ANSHIKA</t>
   </si>
   <si>
     <t>PH3(15B1HS112)- 240/HIM</t>
   </si>
   <si>
-    <t>PF8(24B15EC111)-BE LAB-II/ANG</t>
+    <t>PF8(24B15EC111)-BE LAB-II/ANG/RAS</t>
   </si>
   <si>
     <t>LF24F25(15B11CI111) -111/SANTOSH</t>
   </si>
   <si>
-    <t>PF3(24B15EC111)-/BE LAB-I/VAT</t>
+    <t>TE1(15B11MA111)-118/PKR</t>
+  </si>
+  <si>
+    <t>PF3(24B15EC111)-/BE LAB-I/VAT/ASG</t>
   </si>
   <si>
     <t>PF14(15B1HS112)-246/NIC</t>
@@ -603,7 +599,7 @@
     <t>PF11F12H2(18B15GE111)/EDD/CADD03/HAB/RAK/SUM/JUGENDRA SINGH</t>
   </si>
   <si>
-    <t>PF9(24B15EC111)-/DE LAB/VKM</t>
+    <t>PF9(24B15EC111)-/DE LAB/VKM/DKA</t>
   </si>
   <si>
     <t>LF9F10(15B11MA111)-148
@@ -628,7 +624,7 @@
     <t>LF1F2(15B11HS112) -117/DEV</t>
   </si>
   <si>
-    <t>LE3E4(15B11PH111) -SR05/SHALU</t>
+    <t>LE3E4(15B11PH111) -SR05/URS</t>
   </si>
   <si>
     <t>PF1(15B1HS112)-240/AKS</t>
@@ -657,7 +653,7 @@
 NFMATHS3</t>
   </si>
   <si>
-    <t>LH3H4(15B11PH111) -117/BHARTI</t>
+    <t>LH3H4(15B11PH111) -117/BHT</t>
   </si>
   <si>
     <t>LE3E4(15B11MA111)-123
@@ -712,11 +708,14 @@
     <t>TF13(15B11CI1111) -126/ANK</t>
   </si>
   <si>
-    <t>TE2(15B11PH111) -116
-/SHALU</t>
-  </si>
-  <si>
-    <t>TE1(15B11MA111)-116/PKR</t>
+    <t>TE2(15B11PH111) -116/ADV</t>
+  </si>
+  <si>
+    <t>TE4(15B11MA111)-121
+/ASP</t>
+  </si>
+  <si>
+    <t>TH1(15B11CI111)-118/GAH</t>
   </si>
   <si>
     <t>TE2(15B11MA111)-121
@@ -726,16 +725,12 @@
     <t>TF21(15B11CI1111) -127/SAP</t>
   </si>
   <si>
-    <t>TE4(15B11MA111)-121
-/ASP</t>
+    <t>TF10(15B11PH111)-126/ANK</t>
   </si>
   <si>
     <t>TF25(15B11CI111) -116/JYOTI</t>
   </si>
   <si>
-    <t>TF10(15B11PH111)-126/ANK</t>
-  </si>
-  <si>
     <t>TH1(15B11MA111)-111/PKS</t>
   </si>
   <si>
@@ -746,9 +741,6 @@
   </si>
   <si>
     <t>TF12(15B11CI1111) -116/ARJ</t>
-  </si>
-  <si>
-    <t>TF1(15B11MA111)-116/KKS</t>
   </si>
   <si>
     <t>TF6(24B11EC111)-116/PRK</t>
@@ -783,22 +775,22 @@
     <t>TH3(24B11EC111)-127/BAB</t>
   </si>
   <si>
-    <t>PF12(15B17PH171) -41//SKA/BHARTI</t>
-  </si>
-  <si>
-    <t>PE4(15B17PH171) -41//ADV/PC</t>
+    <t>PF12(15B17PH171) -41//SKH</t>
+  </si>
+  <si>
+    <t>PE4(15B17PH171) -41/ADV</t>
   </si>
   <si>
     <t>LF5F6(15B11HS112) -118/NIC</t>
   </si>
   <si>
-    <t>PF5(15B17PH171)-027//BHARTI/SKH</t>
+    <t>PF5(15B17PH171)-256C/NAK</t>
   </si>
   <si>
     <t>PE2(15B1HS112)-246//DEV</t>
   </si>
   <si>
-    <t>PH4(15B17PH171)-027//BHARTI/NFPHY3</t>
+    <t>PH4(15B17PH171)-256C/BHT</t>
   </si>
   <si>
     <t>TF17(15B11MA111)-116/SHP</t>
@@ -810,7 +802,7 @@
     <t>TF25(15B11MA111)-121/ASP</t>
   </si>
   <si>
-    <t>PF13F14H3(18B15GE111) -EDD/CADD03/PSH/RAK/HAB</t>
+    <t>PF13F14H3(18B15GE111) -EDD/CADD03/PSH/RAK/HAB/JUGENDRA SINGH</t>
   </si>
   <si>
     <t>LH1H2(24B11EC111) -117 
@@ -820,23 +812,23 @@
     <t>PE1E2H4(18B15GE111)/EDD/CADD03/NIK/PRJ/SUM/RAVI</t>
   </si>
   <si>
-    <t>PF11(15B17PH171)-027/AMV</t>
+    <t>PF11(15B17PH171)-256C/AMV</t>
   </si>
   <si>
     <t>LF21F22(24B11EC111) -148 
 /RPV</t>
   </si>
   <si>
-    <t>TE3(15B11PH111)-121/NFPHY2</t>
-  </si>
-  <si>
-    <t>PF13F14H1(24B15CS111)--CL1/TWT/HIB/SANTOSH</t>
-  </si>
-  <si>
-    <t>TF18(15B11PH111)-126/BHARTI</t>
-  </si>
-  <si>
-    <t>PE4F18F17(24B15CS111)-CL1/ANKIT/SHM/TWT</t>
+    <t>TE3(15B11PH111)-121/ADV</t>
+  </si>
+  <si>
+    <t>PF13F14H1(24B15CS111)--CL1/TWT/HIB/SANTOSH/BAIBHAV</t>
+  </si>
+  <si>
+    <t>TF18(15B11PH111)-126/KAS</t>
+  </si>
+  <si>
+    <t>PE4F18F17(24B15CS111)-CL1/ANKIT/SHM/TWT/SAMARTH JAIN</t>
   </si>
   <si>
     <t>LF21F22(15B11CI1111) -148 /SAP</t>
@@ -846,13 +838,13 @@
 /KUM</t>
   </si>
   <si>
-    <t>LF21F22(15B11PH111) -117/VM</t>
-  </si>
-  <si>
-    <t>PF22(24B15EC111)-/DE LAB/KDT</t>
-  </si>
-  <si>
-    <t>PF18(24B15EC111)/BE LAB-II/ABK</t>
+    <t>LF21F22(15B11PH111) -117/KAS</t>
+  </si>
+  <si>
+    <t>PF22(24B15EC111)-/DE LAB/KDT/AJK</t>
+  </si>
+  <si>
+    <t>PF18(24B15EC111)/BE LAB-II/ABK/MEA</t>
   </si>
   <si>
     <t>LF18F17(15B11CI1111) -111 
@@ -862,7 +854,7 @@
     <t>TF12(15B11MA111)-127/SHP</t>
   </si>
   <si>
-    <t>PH1(24B15EC111)-BE LAB-I/PAA</t>
+    <t>PH1(24B15EC111)-BE LAB-I/PAA/RKS</t>
   </si>
   <si>
     <t>LF7F8(15B11MA111)-118
@@ -885,7 +877,7 @@
     <t>LF9F10(15B11PH111) -123/ANK</t>
   </si>
   <si>
-    <t>TF17(15B11PH111)-111/BHARTI</t>
+    <t>TF17(15B11PH111)-111/BHT</t>
   </si>
   <si>
     <t>LF9F10(15B11CI1111) -123 /JYOTI</t>
@@ -904,22 +896,19 @@
     <t>TF11(15B11PH111)-123/SKH</t>
   </si>
   <si>
-    <t>TH1(15B11CI1111) -116/GAH</t>
-  </si>
-  <si>
     <t>LF7F8(15B11PH111) -118/URS</t>
   </si>
   <si>
     <t>TF4(15B11CI1111) -116/AVINASH</t>
   </si>
   <si>
-    <t>TH3(15B11PH111)-121/NAK</t>
-  </si>
-  <si>
-    <t>PF24(15B17PH171)-41/NFPHY2</t>
-  </si>
-  <si>
-    <t>TF5(15B11PH111)-121/ADV</t>
+    <t>TH3(15B11PH111)-121/KAS</t>
+  </si>
+  <si>
+    <t>PF24(15B17PH171)-41/SHALU</t>
+  </si>
+  <si>
+    <t>TF5(15B11PH111)-121/SHALU</t>
   </si>
   <si>
     <t>TF2(15B11CI1111) -121/VIS</t>
@@ -928,10 +917,10 @@
     <t>TF17(15B11CI1111) -121/DEEPTI</t>
   </si>
   <si>
-    <t>PH3(24B15EC111)/BE LAB II/ABK</t>
-  </si>
-  <si>
-    <t>TH2(15B11PH111)-116/SKA</t>
+    <t>PH3(24B15EC111)/BE LAB II/ABK/BHC</t>
+  </si>
+  <si>
+    <t>TH2(15B11PH111)-116/KAS</t>
   </si>
   <si>
     <t>TF7(15B11MA111)-126 /MSZ</t>
@@ -943,22 +932,28 @@
     <t>TF9(15B11PH111)-118/ANK</t>
   </si>
   <si>
-    <t>TH4(15B11PH111)-127/NAK</t>
-  </si>
-  <si>
-    <t>TF8(15B11MA111)-127/PKS</t>
+    <t>TF24(15B11CI111) -126/JYOTI</t>
+  </si>
+  <si>
+    <t>TH4(15B11PH111)-127/VM</t>
+  </si>
+  <si>
+    <t>TF8(15B11MA111)-127/NFMATHS1</t>
   </si>
   <si>
     <t>TF3(15B11MA111)-SR05/NEA</t>
   </si>
   <si>
-    <t>PF25(24B15CS111)-CL4/SANTOSH</t>
+    <t>PF25(24B15CS111)-CL4/SANTOSH/JATIN</t>
   </si>
   <si>
     <t>TF1(24B11EC111)-123/BHC</t>
   </si>
   <si>
     <t>FRIDAY</t>
+  </si>
+  <si>
+    <t>TF7(15B11CI1111) -127/ADS</t>
   </si>
   <si>
     <t>TF22(15B11MA111)-116/ASP</t>
@@ -989,17 +984,13 @@
     <t>TF6(15B11MA111)-121/MSZ</t>
   </si>
   <si>
-    <t>PF21(15B17PH171) -027//SKA/NFPHY2</t>
-  </si>
-  <si>
-    <t>PF22(15B17PH171)-41//AMV/ANK</t>
-  </si>
-  <si>
-    <t>PF18(15B17PH171)-027//ANK/SKA</t>
-  </si>
-  <si>
-    <t>LF24F25(15B11PH111) -123
-/NFPHY2</t>
+    <t>PF21(15B17PH171) -41/KAS/VM</t>
+  </si>
+  <si>
+    <t>PF22(15B17PH171)-256C/AMV</t>
+  </si>
+  <si>
+    <t>PF18(15B17PH171)-41/ANK</t>
   </si>
   <si>
     <t>PE3E4(18B15GE111)/EDD/CADD03/PRJ/NIK/RAVI</t>
@@ -1013,10 +1004,10 @@
 /PKR</t>
   </si>
   <si>
-    <t>PF9F10H1(18B15GE111)/EDD/CADD03/SUM/RAK/PSH/JUGENDRA SINGH</t>
-  </si>
-  <si>
-    <t>PF13(24B15EC111)-BE LAB-I/NIY</t>
+    <t>PF9F10H1(18B15GE111)/EDD/CADD03/SUM/RAK/PSH</t>
+  </si>
+  <si>
+    <t>PF13(24B15EC111)-BE LAB-I/NIY/KUM</t>
   </si>
   <si>
     <t>LF18F17(24B11EC111) -117 /RPV</t>
@@ -1026,32 +1017,32 @@
 /BAB</t>
   </si>
   <si>
-    <t>PE1E2E3(24B15CS111)-CL1/ARJ/SHM/TKW/NFCS1</t>
+    <t>PE1E2E3(24B15CS111)-CL1/ARJ/SHM/DEEPTI/BAIBHAV</t>
   </si>
   <si>
     <t>TF12(24B11EC111)-126/RUS</t>
   </si>
   <si>
-    <t>PF14(24B15EC111)-DE LAB/VKM</t>
+    <t>PF14(24B15EC111)-DE LAB/VKM/AJK</t>
   </si>
   <si>
     <t>LF9F10(24B11EC111) -123
 /KUM</t>
   </si>
   <si>
+    <t>PF11(15B1HS112)-246/NIC</t>
+  </si>
+  <si>
     <t>TF2(15B11MA111))-116/KKS</t>
   </si>
   <si>
-    <t>PF11(15B1HS112)-246/NIC</t>
-  </si>
-  <si>
     <t>LF1F2(24B11EC111) -123/BHC</t>
   </si>
   <si>
     <t>LH1H2(15B11CI1111) - SR05/GAH</t>
   </si>
   <si>
-    <t>PE2(24B15EC111) -/BE LAB-II/AJK</t>
+    <t>PE2(24B15EC111) -/BE LAB-II/AJK/PAA</t>
   </si>
   <si>
     <t>TF21(24B11EC111)-121/RPV</t>
@@ -1101,7 +1092,7 @@
 /BAB</t>
   </si>
   <si>
-    <t>TF6(15B11PH111)-121/URS</t>
+    <t>TF6(15B11PH111)-121/SHALU</t>
   </si>
   <si>
     <t>TH4(24B11EC111) -116/BAB</t>
@@ -1132,7 +1123,7 @@
     <t>TF14(15B11CI1111) -116/ANK</t>
   </si>
   <si>
-    <t>LF21F22(15B11PH111) -123/VM</t>
+    <t>LF21F22(15B11PH111) -123/KAS</t>
   </si>
   <si>
     <t>PF24(15B1HS112)-246/MEENAKSHI/ANSHIKA</t>
@@ -1141,16 +1132,16 @@
     <t>LF1F2(15B11PH111) -SR05/AMV</t>
   </si>
   <si>
-    <t>PF25(15B17PH171)-027/NFPHY2</t>
-  </si>
-  <si>
-    <t>PF25(15B1HS112)-240/HIMANSHI/RACHNA</t>
+    <t>PF25(15B17PH171)-0256C/SHALU</t>
+  </si>
+  <si>
+    <t>PF25(15B1HS112)-240/SHV</t>
   </si>
   <si>
     <t>TF13(15B11PH111)-121/NAK</t>
   </si>
   <si>
-    <t>PF24(24B15CS111) - /CL1//RISHAB NEGI</t>
+    <t>PF24(24B15CS111) - /CL1/JATIN/RISHAB NEGI</t>
   </si>
   <si>
     <t>SATURDAY</t>
@@ -1184,16 +1175,13 @@
 /PRK</t>
   </si>
   <si>
-    <t>PE4(24B15EC111)/BE LAB-II/DKA</t>
+    <t>PE4(24B15EC111)/BE LAB-II/DKA/RAS</t>
   </si>
   <si>
     <t>LF13F14(15B11CI1111)-3023 
 /ANKIT</t>
   </si>
   <si>
-    <t>LF1F2(24B11CI111) - 3040/VIS</t>
-  </si>
-  <si>
     <t>LH1H2(15B11CI1111) -3028
 /GAH</t>
   </si>
@@ -1230,6 +1218,9 @@
     <t>LE1E2(24B11EC111) -111 /PRK</t>
   </si>
   <si>
+    <t>LF1F2(24B11CI111) - 3040/VIS</t>
+  </si>
+  <si>
     <t>LH3H4(24B11EC111) -123 /BAB</t>
   </si>
   <si>
@@ -1241,7 +1232,8 @@
 /PKR</t>
   </si>
   <si>
-    <t>LF18F17(15B11HS112) -148//DEV</t>
+    <t>LF18F17(15B11HS112) -148
+//CHANDRESHEKHAR</t>
   </si>
   <si>
     <t>LF9F10(15B11CI1111) -138 /JYOTI</t>
@@ -1261,22 +1253,19 @@
     <t>LF13F14(24B11EC111) - 3023/ATK</t>
   </si>
   <si>
-    <t>TF2(15B11PH111)-126/URS</t>
+    <t>TF2(15B11PH111)-126/AMV</t>
   </si>
   <si>
     <t>LF7F8(15B11PH111) -3028/URS</t>
   </si>
   <si>
-    <t>TF7(15B11CI1111) -127/ADS</t>
+    <t>TF18(15B11MA111)-113/PKS</t>
   </si>
   <si>
     <t>LF1F2(15B11PH111) -3040/AMV</t>
   </si>
   <si>
-    <t>TF18(15B11MA111)-113/PKS</t>
-  </si>
-  <si>
-    <t>PF24(18B15GE111)/EDD/CADD03/RAK</t>
+    <t>PF24(18B15GE111)/EDD/CADD03/HAB</t>
   </si>
   <si>
     <t>PF25(18B15GE111)/EDD/CADD03/PSH</t>
@@ -1786,10 +1775,10 @@
     <t>25</t>
   </si>
   <si>
-    <t>TKW</t>
-  </si>
-  <si>
-    <t>Tarkeshwar</t>
+    <t>JATIN</t>
+  </si>
+  <si>
+    <t>Jatin</t>
   </si>
   <si>
     <t>54</t>
@@ -1873,10 +1862,28 @@
     <t>Shivani Pant</t>
   </si>
   <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>JYOTI</t>
+  </si>
+  <si>
+    <t>Jyoti</t>
+  </si>
+  <si>
     <t>VIS</t>
   </si>
   <si>
     <t>Vikas Sharma</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>BAIBHAV</t>
+  </si>
+  <si>
+    <t>Baibhav</t>
   </si>
 </sst>
 </file>
@@ -2131,15 +2138,15 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="31.43"/>
-    <col customWidth="1" min="2" max="2" width="53.14"/>
-    <col customWidth="1" min="3" max="3" width="42.0"/>
-    <col customWidth="1" min="4" max="4" width="41.43"/>
-    <col customWidth="1" min="5" max="5" width="41.14"/>
-    <col customWidth="1" min="6" max="6" width="52.14"/>
-    <col customWidth="1" min="7" max="7" width="62.0"/>
-    <col customWidth="1" min="8" max="8" width="54.43"/>
-    <col customWidth="1" min="9" max="9" width="89.86"/>
+    <col customWidth="1" min="1" max="1" width="33.14"/>
+    <col customWidth="1" min="2" max="2" width="47.0"/>
+    <col customWidth="1" min="3" max="3" width="38.43"/>
+    <col customWidth="1" min="4" max="4" width="50.86"/>
+    <col customWidth="1" min="5" max="5" width="42.29"/>
+    <col customWidth="1" min="6" max="6" width="53.29"/>
+    <col customWidth="1" min="7" max="7" width="51.71"/>
+    <col customWidth="1" min="8" max="8" width="45.57"/>
+    <col customWidth="1" min="9" max="9" width="45.43"/>
     <col customWidth="1" min="10" max="26" width="8.71"/>
   </cols>
   <sheetData>
@@ -2642,242 +2649,241 @@
         <v>140</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="B37" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="B38" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="D39" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
+    </row>
+    <row r="39" ht="15.75" customHeight="1"/>
     <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="D42" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="B43" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="B44" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="B45" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="B46" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="B47" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="B48" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="B49" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="B50" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="B51" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="B52" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
@@ -2885,35 +2891,38 @@
         <v>31</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="H53" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="B54" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="G54" s="1" t="s">
+      <c r="H54" s="1" t="s">
         <v>219</v>
       </c>
     </row>
@@ -2936,290 +2945,284 @@
         <v>224</v>
       </c>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="G57" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
+    <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1"/>
     <row r="59" ht="15.75" customHeight="1"/>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="D61" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="H61" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="G61" s="1" t="s">
+      <c r="I61" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="B62" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="F62" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="G62" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="H62" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G62" s="1" t="s">
+      <c r="I62" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="B63" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="G63" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="B64" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="G64" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="I64" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="B65" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="B66" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>119</v>
       </c>
       <c r="E66" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="I66" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="B67" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="F67" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="B68" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G68" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="H68" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="B69" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="H69" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="C70" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="G70" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="H70" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="B71" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="G71" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="H71" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="G71" s="1" t="s">
+    </row>
+    <row r="72" ht="15.75" customHeight="1">
+      <c r="C72" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H71" s="1" t="s">
+      <c r="D72" s="1" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="72" ht="15.75" customHeight="1">
-      <c r="B72" s="1" t="s">
+      <c r="E72" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="G72" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="B73" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G73" s="1" t="s">
         <v>283</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="B74" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="H74" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="B75" s="1" t="s">
-        <v>153</v>
+        <v>288</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H75" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="B76" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="B77" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1"/>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="80" ht="15.75" customHeight="1"/>
+        <v>294</v>
+      </c>
+    </row>
+    <row r="80" ht="15.75" customHeight="1">
+      <c r="D80" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="C81" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="G81" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="G81" s="1" t="s">
+      <c r="I81" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="I81" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="82" ht="15.75" customHeight="1">
@@ -3230,104 +3233,104 @@
         <v>33</v>
       </c>
       <c r="D82" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="G82" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="G82" s="1" t="s">
+      <c r="H82" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="H82" s="1" t="s">
+      <c r="I82" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="I82" s="1" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="B83" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="F83" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>308</v>
-      </c>
       <c r="I83" s="1" t="s">
-        <v>309</v>
+        <v>131</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="B84" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="G84" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="B85" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>316</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>121</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="B86" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G86" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E86" s="1" t="s">
+      <c r="I86" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="B87" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="F87" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="G87" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="88" ht="15.75" customHeight="1">
@@ -3335,115 +3338,115 @@
         <v>32</v>
       </c>
       <c r="C88" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="F88" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="G88" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="F88" s="1" t="s">
+      <c r="H88" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="B89" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="E89" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="F89" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="G89" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="F89" s="1" t="s">
+      <c r="H89" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="B90" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="E90" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="G90" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="H90" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="H90" s="1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="B91" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>349</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>53</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="D92" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="B93" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G93" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>355</v>
-      </c>
       <c r="H93" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="B94" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1"/>
@@ -3453,842 +3456,857 @@
     <row r="99" ht="15.75" customHeight="1"/>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="C101" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E101" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="B102" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E102" s="1" t="s">
         <v>361</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="B103" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E103" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="B104" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="B105" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>369</v>
+        <v>258</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="B106" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E106" s="1" t="s">
         <v>371</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="B107" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E107" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="B108" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="E108" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="B109" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="E109" s="1" t="s">
         <v>383</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="B110" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D110" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="E110" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="D111" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="D112" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="C113" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1">
       <c r="C114" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1"/>
     <row r="116" ht="15.75" customHeight="1"/>
     <row r="117" ht="15.75" customHeight="1">
       <c r="B117" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="H117" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="I117" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="H117" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="I117" s="1" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
       <c r="B118" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="E118" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="F118" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="G118" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="E118" s="1" t="s">
+      <c r="H118" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="F118" s="1" t="s">
+      <c r="I118" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="G118" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="H118" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="I118" s="1" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
       <c r="B119" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="E119" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="F119" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="G119" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="E119" s="1" t="s">
+      <c r="H119" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="F119" s="1" t="s">
+      <c r="I119" s="1" t="s">
         <v>413</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="H119" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="I119" s="1" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1">
       <c r="B120" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="E120" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="F120" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="G120" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="E120" s="1" t="s">
+      <c r="H120" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="F120" s="1" t="s">
+      <c r="I120" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="G120" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="H120" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="I120" s="1" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="121" ht="15.75" customHeight="1">
       <c r="B121" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E121" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="F121" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="G121" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="E121" s="1" t="s">
+      <c r="H121" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="F121" s="1" t="s">
+      <c r="I121" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="G121" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="H121" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="I121" s="1" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1">
       <c r="B122" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="E122" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="F122" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="G122" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="E122" s="1" t="s">
+      <c r="H122" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="F122" s="1" t="s">
+      <c r="I122" s="1" t="s">
         <v>437</v>
-      </c>
-      <c r="G122" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="H122" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="I122" s="1" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="123" ht="15.75" customHeight="1">
       <c r="B123" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="E123" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="F123" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="G123" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="E123" s="1" t="s">
+      <c r="H123" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="F123" s="1" t="s">
+      <c r="I123" s="1" t="s">
         <v>445</v>
-      </c>
-      <c r="G123" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="H123" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="I123" s="1" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="124" ht="15.75" customHeight="1">
       <c r="B124" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="E124" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="F124" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="G124" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E124" s="1" t="s">
+      <c r="H124" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="F124" s="1" t="s">
+      <c r="I124" s="1" t="s">
         <v>453</v>
-      </c>
-      <c r="G124" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="H124" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="I124" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="125" ht="15.75" customHeight="1">
       <c r="B125" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="E125" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="F125" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="G125" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="E125" s="1" t="s">
+      <c r="H125" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="F125" s="1" t="s">
+      <c r="I125" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="G125" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="H125" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="I125" s="1" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1">
       <c r="B126" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="E126" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="F126" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="G126" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="E126" s="1" t="s">
+      <c r="H126" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="F126" s="1" t="s">
+      <c r="I126" s="1" t="s">
         <v>469</v>
-      </c>
-      <c r="G126" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="H126" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="I126" s="1" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
       <c r="B127" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="E127" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="F127" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="D127" s="1" t="s">
+      <c r="G127" s="1" t="s">
         <v>475</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="128" ht="15.75" customHeight="1">
       <c r="B128" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="E128" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="F128" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="D128" s="1" t="s">
+      <c r="G128" s="1" t="s">
         <v>481</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="G128" s="1" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
       <c r="B129" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="E129" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="F129" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="D129" s="1" t="s">
+      <c r="G129" s="1" t="s">
         <v>487</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="G129" s="1" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
       <c r="B130" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="E130" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="F130" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="D130" s="1" t="s">
+      <c r="G130" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="G130" s="1" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="131" ht="15.75" customHeight="1">
       <c r="B131" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="E131" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="F131" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="D131" s="1" t="s">
+      <c r="G131" s="1" t="s">
         <v>499</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="G131" s="1" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="132" ht="15.75" customHeight="1">
       <c r="B132" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="E132" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="F132" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="G132" s="1" t="s">
         <v>505</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="G132" s="1" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="133" ht="15.75" customHeight="1">
       <c r="B133" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="E133" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="F133" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="D133" s="1" t="s">
+      <c r="G133" s="1" t="s">
         <v>511</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="F133" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="G133" s="1" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="134" ht="15.75" customHeight="1">
       <c r="B134" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="E134" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="F134" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="G134" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="F134" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="G134" s="1" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="135" ht="15.75" customHeight="1">
       <c r="B135" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="E135" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="F135" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="D135" s="1" t="s">
+      <c r="G135" s="1" t="s">
         <v>523</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="G135" s="1" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="136" ht="15.75" customHeight="1">
       <c r="B136" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="E136" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="F136" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="D136" s="1" t="s">
+      <c r="G136" s="1" t="s">
         <v>529</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="137" ht="15.75" customHeight="1">
       <c r="B137" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="E137" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="F137" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="D137" s="1" t="s">
+      <c r="G137" s="1" t="s">
         <v>535</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="G137" s="1" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="138" ht="15.75" customHeight="1">
       <c r="B138" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="E138" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="C138" s="1" t="s">
+      <c r="F138" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="D138" s="1" t="s">
+      <c r="G138" s="1" t="s">
         <v>541</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="139" ht="15.75" customHeight="1">
       <c r="B139" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="E139" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="F139" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="D139" s="1" t="s">
+      <c r="G139" s="1" t="s">
         <v>547</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="G139" s="1" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="140" ht="15.75" customHeight="1">
       <c r="B140" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="E140" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="C140" s="1" t="s">
+      <c r="F140" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="D140" s="1" t="s">
+      <c r="G140" s="1" t="s">
         <v>553</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="F140" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="141" ht="15.75" customHeight="1">
       <c r="B141" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="E141" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="F141" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="D141" s="1" t="s">
+      <c r="G141" s="1" t="s">
         <v>559</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>560</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>561</v>
-      </c>
-      <c r="G141" s="1" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="142" ht="15.75" customHeight="1">
       <c r="B142" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="E142" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="F142" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="D142" s="1" t="s">
+      <c r="G142" s="1" t="s">
         <v>565</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="F142" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="G142" s="1" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="143" ht="15.75" customHeight="1">
       <c r="B143" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="E143" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="F143" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="D143" s="1" t="s">
+      <c r="G143" s="1" t="s">
         <v>571</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="G143" s="1" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="144" ht="15.75" customHeight="1">
       <c r="B144" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="E144" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="C144" s="1" t="s">
-        <v>576</v>
-      </c>
-      <c r="D144" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>578</v>
-      </c>
       <c r="F144" s="1" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="145" ht="15.75" customHeight="1">
       <c r="B145" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="E145" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="F145" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="D145" s="1" t="s">
+      <c r="G145" s="1" t="s">
         <v>581</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>582</v>
-      </c>
-      <c r="F145" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="146" ht="15.75" customHeight="1">
       <c r="B146" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="E146" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="F146" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="D146" s="1" t="s">
+      <c r="G146" s="1" t="s">
         <v>587</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="G146" s="1" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="147" ht="15.75" customHeight="1">
       <c r="B147" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C147" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="F147" s="1" t="s">
         <v>591</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="G147" s="1" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="148" ht="15.75" customHeight="1">
       <c r="B148" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>593</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>594</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="149" ht="15.75" customHeight="1"/>
@@ -5123,130 +5141,129 @@
     <row r="978" ht="15.75" customHeight="1"/>
     <row r="979" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="123">
-    <mergeCell ref="D7:E7"/>
+  <mergeCells count="122">
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="A3:A20"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="C113:E113"/>
+    <mergeCell ref="A100:A116"/>
+    <mergeCell ref="F100:I116"/>
+    <mergeCell ref="C114:E114"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="A60:A78"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="G87:H87"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="G84:I84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="G85:H85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="D87:E87"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B49:C49"/>
     <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="A60:A78"/>
+    <mergeCell ref="A21:A40"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="A41:A59"/>
     <mergeCell ref="A79:A99"/>
-    <mergeCell ref="A100:A116"/>
-    <mergeCell ref="A117:A139"/>
-    <mergeCell ref="A140:A148"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="A117:A148"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
     <mergeCell ref="B93:C93"/>
     <mergeCell ref="B94:C94"/>
     <mergeCell ref="B102:C102"/>
     <mergeCell ref="B103:C103"/>
     <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="D45:E45"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="F46:G46"/>
-    <mergeCell ref="B47:C47"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="F47:G47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="G65:I65"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="G59:H59"/>
     <mergeCell ref="D83:E83"/>
     <mergeCell ref="G83:H83"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="G84:I84"/>
-    <mergeCell ref="C113:E113"/>
-    <mergeCell ref="C114:E114"/>
-    <mergeCell ref="E148:G148"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="G87:H87"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="F100:I116"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A3:A20"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="A21:A40"/>
-    <mergeCell ref="A41:A59"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G59:H59"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>

</xml_diff>